<commit_message>
strat empty templates with 2025 labeling
</commit_message>
<xml_diff>
--- a/CIS_Template_Strat.xlsx
+++ b/CIS_Template_Strat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshua.mcdonald\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usradiology-my.sharepoint.com/personal/joshua_mcdonald_usradiology_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1897A65-81C7-489D-81E6-BC1D9344331E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2957D2B7-9833-40D8-B748-A1FF54E0818A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="777" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="777" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary (with DeNovo)" sheetId="22" r:id="rId1"/>
@@ -52,42 +52,6 @@
     <t>DEXA</t>
   </si>
   <si>
-    <t>Jan24</t>
-  </si>
-  <si>
-    <t>Feb24</t>
-  </si>
-  <si>
-    <t>Mar24</t>
-  </si>
-  <si>
-    <t>Apr24</t>
-  </si>
-  <si>
-    <t>May24</t>
-  </si>
-  <si>
-    <t>Jun24</t>
-  </si>
-  <si>
-    <t>Jul24</t>
-  </si>
-  <si>
-    <t>Aug24</t>
-  </si>
-  <si>
-    <t>Sep24</t>
-  </si>
-  <si>
-    <t>Oct24</t>
-  </si>
-  <si>
-    <t>Nov24</t>
-  </si>
-  <si>
-    <t>Dec24</t>
-  </si>
-  <si>
     <t>CT</t>
   </si>
   <si>
@@ -110,6 +74,42 @@
   </si>
   <si>
     <t>Screening Mamm</t>
+  </si>
+  <si>
+    <t>Jan25</t>
+  </si>
+  <si>
+    <t>Feb25</t>
+  </si>
+  <si>
+    <t>Mar25</t>
+  </si>
+  <si>
+    <t>Apr25</t>
+  </si>
+  <si>
+    <t>May25</t>
+  </si>
+  <si>
+    <t>Jun25</t>
+  </si>
+  <si>
+    <t>Jul25</t>
+  </si>
+  <si>
+    <t>Aug25</t>
+  </si>
+  <si>
+    <t>Sep25</t>
+  </si>
+  <si>
+    <t>Oct25</t>
+  </si>
+  <si>
+    <t>Nov25</t>
+  </si>
+  <si>
+    <t>Dec25</t>
   </si>
 </sst>
 </file>
@@ -481,14 +481,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,48 +496,48 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <f>Ballantyne!C2+Denver!C2+Huntersville!C2+Matthews!C2+'Rock Hill'!C2+Southpark!C2+FortMill!C2</f>
@@ -588,12 +588,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <f>Ballantyne!C3+Denver!C3+Huntersville!C3+Matthews!C3+'Rock Hill'!C3+Southpark!C3+FortMill!C3</f>
@@ -644,12 +644,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <f>Ballantyne!C4+Denver!C4+Huntersville!C4+Matthews!C4+'Rock Hill'!C4+Southpark!C4+FortMill!C4</f>
@@ -700,12 +700,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <f>Ballantyne!C5+Denver!C5+Huntersville!C5+Matthews!C5+'Rock Hill'!C5+Southpark!C5+FortMill!C5</f>
@@ -756,12 +756,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <f>Ballantyne!C6+Denver!C6+Huntersville!C6+Matthews!C6+'Rock Hill'!C6+Southpark!C6+FortMill!C6</f>
@@ -812,12 +812,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <f>Ballantyne!C7+Denver!C7+Huntersville!C7+Matthews!C7+'Rock Hill'!C7+Southpark!C7+FortMill!C7</f>
@@ -868,12 +868,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <f>Ballantyne!C8+Denver!C8+Huntersville!C8+Matthews!C8+'Rock Hill'!C8+Southpark!C8+FortMill!C8</f>
@@ -924,12 +924,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <f>Ballantyne!C9+Denver!C9+Huntersville!C9+Matthews!C9+'Rock Hill'!C9+Southpark!C9+FortMill!C9</f>
@@ -980,7 +980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1047,14 +1047,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1062,48 +1062,48 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <f>Ballantyne!C2+Denver!C2+Huntersville!C2+Matthews!C2+'Rock Hill'!C2+Southpark!C2</f>
@@ -1154,12 +1154,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <f>Ballantyne!C3+Denver!C3+Huntersville!C3+Matthews!C3+'Rock Hill'!C3+Southpark!C3</f>
@@ -1210,12 +1210,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <f>Ballantyne!C4+Denver!C4+Huntersville!C4+Matthews!C4+'Rock Hill'!C4+Southpark!C4</f>
@@ -1266,12 +1266,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <f>Ballantyne!C5+Denver!C5+Huntersville!C5+Matthews!C5+'Rock Hill'!C5+Southpark!C5</f>
@@ -1322,12 +1322,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <f>Ballantyne!C6+Denver!C6+Huntersville!C6+Matthews!C6+'Rock Hill'!C6+Southpark!C6</f>
@@ -1378,12 +1378,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <f>Ballantyne!C7+Denver!C7+Huntersville!C7+Matthews!C7+'Rock Hill'!C7+Southpark!C7</f>
@@ -1434,12 +1434,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <f>Ballantyne!C8+Denver!C8+Huntersville!C8+Matthews!C8+'Rock Hill'!C8+Southpark!C8</f>
@@ -1490,12 +1490,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <f>Ballantyne!C9+Denver!C9+Huntersville!C9+Matthews!C9+'Rock Hill'!C9+Southpark!C9</f>
@@ -1546,7 +1546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1613,14 +1613,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1628,107 +1628,107 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
       <c r="B9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1747,14 +1747,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1762,107 +1762,107 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
       <c r="B9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1881,14 +1881,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1896,107 +1896,107 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
       <c r="B9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -2015,14 +2015,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2030,107 +2030,107 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
       <c r="B9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -2149,14 +2149,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2164,107 +2164,107 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
       <c r="B9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -2283,14 +2283,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2298,107 +2298,107 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
       <c r="B9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -2417,14 +2417,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2432,107 +2432,107 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
       <c r="B9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
update CIS template strat plan 2026
</commit_message>
<xml_diff>
--- a/CIS_Template_Strat.xlsx
+++ b/CIS_Template_Strat.xlsx
@@ -1,27 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usradiology-my.sharepoint.com/personal/joshua_mcdonald_usradiology_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2957D2B7-9833-40D8-B748-A1FF54E0818A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0903A04-6BF9-4505-99FE-84648EA2B62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="777" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="777" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary (with DeNovo)" sheetId="22" r:id="rId1"/>
     <sheet name="Summary (no DeNovo)" sheetId="20" r:id="rId2"/>
     <sheet name="Ballantyne" sheetId="2" r:id="rId3"/>
     <sheet name="Denver" sheetId="3" r:id="rId4"/>
-    <sheet name="Huntersville" sheetId="4" r:id="rId5"/>
-    <sheet name="Matthews" sheetId="5" r:id="rId6"/>
-    <sheet name="Rock Hill" sheetId="14" r:id="rId7"/>
-    <sheet name="Southpark" sheetId="16" r:id="rId8"/>
-    <sheet name="FortMill" sheetId="21" r:id="rId9"/>
+    <sheet name="FortMill" sheetId="21" r:id="rId5"/>
+    <sheet name="Huntersville" sheetId="4" r:id="rId6"/>
+    <sheet name="Matthews" sheetId="5" r:id="rId7"/>
+    <sheet name="Rock Hill" sheetId="14" r:id="rId8"/>
+    <sheet name="Southpark" sheetId="16" r:id="rId9"/>
+    <sheet name="Concord" sheetId="23" r:id="rId10"/>
+    <sheet name="Indian Trail" sheetId="24" r:id="rId11"/>
+    <sheet name="OtherDeNovo" sheetId="25" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="24">
   <si>
     <t>ExamCategory</t>
   </si>
@@ -76,40 +79,43 @@
     <t>Screening Mamm</t>
   </si>
   <si>
-    <t>Jan25</t>
+    <t>PET/CT</t>
   </si>
   <si>
-    <t>Feb25</t>
+    <t>Jan26</t>
   </si>
   <si>
-    <t>Mar25</t>
+    <t>Feb26</t>
   </si>
   <si>
-    <t>Apr25</t>
+    <t>Mar26</t>
   </si>
   <si>
-    <t>May25</t>
+    <t>Apr26</t>
   </si>
   <si>
-    <t>Jun25</t>
+    <t>May26</t>
   </si>
   <si>
-    <t>Jul25</t>
+    <t>Jun26</t>
   </si>
   <si>
-    <t>Aug25</t>
+    <t>Jul26</t>
   </si>
   <si>
-    <t>Sep25</t>
+    <t>Aug26</t>
   </si>
   <si>
-    <t>Oct25</t>
+    <t>Sep26</t>
   </si>
   <si>
-    <t>Nov25</t>
+    <t>Oct26</t>
   </si>
   <si>
-    <t>Dec25</t>
+    <t>Nov26</t>
+  </si>
+  <si>
+    <t>Dec26</t>
   </si>
 </sst>
 </file>
@@ -168,9 +174,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -477,62 +486,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B0F8F8-48F1-495E-AB27-ABE4AA2E5916}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -540,55 +549,55 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <f>Ballantyne!C2+Denver!C2+Huntersville!C2+Matthews!C2+'Rock Hill'!C2+Southpark!C2+FortMill!C2</f>
+        <f>Ballantyne!C2+Denver!C2+FortMill!C2+Huntersville!C2+Matthews!C2+'Rock Hill'!C2+Southpark!C2+Concord!C2+'Indian Trail'!C2+OtherDeNovo!C2</f>
         <v>0</v>
       </c>
       <c r="D2">
-        <f>Ballantyne!D2+Denver!D2+Huntersville!D2+Matthews!D2+'Rock Hill'!D2+Southpark!D2+FortMill!D2</f>
+        <f>Ballantyne!D2+Denver!D2+FortMill!D2+Huntersville!D2+Matthews!D2+'Rock Hill'!D2+Southpark!D2+Concord!D2+'Indian Trail'!D2+OtherDeNovo!D2</f>
         <v>0</v>
       </c>
       <c r="E2">
-        <f>Ballantyne!E2+Denver!E2+Huntersville!E2+Matthews!E2+'Rock Hill'!E2+Southpark!E2+FortMill!E2</f>
+        <f>Ballantyne!E2+Denver!E2+FortMill!E2+Huntersville!E2+Matthews!E2+'Rock Hill'!E2+Southpark!E2+Concord!E2+'Indian Trail'!E2+OtherDeNovo!E2</f>
         <v>0</v>
       </c>
       <c r="F2">
-        <f>Ballantyne!F2+Denver!F2+Huntersville!F2+Matthews!F2+'Rock Hill'!F2+Southpark!F2+FortMill!F2</f>
+        <f>Ballantyne!F2+Denver!F2+FortMill!F2+Huntersville!F2+Matthews!F2+'Rock Hill'!F2+Southpark!F2+Concord!F2+'Indian Trail'!F2+OtherDeNovo!F2</f>
         <v>0</v>
       </c>
       <c r="G2">
-        <f>Ballantyne!G2+Denver!G2+Huntersville!G2+Matthews!G2+'Rock Hill'!G2+Southpark!G2+FortMill!G2</f>
+        <f>Ballantyne!G2+Denver!G2+FortMill!G2+Huntersville!G2+Matthews!G2+'Rock Hill'!G2+Southpark!G2+Concord!G2+'Indian Trail'!G2+OtherDeNovo!G2</f>
         <v>0</v>
       </c>
       <c r="H2">
-        <f>Ballantyne!H2+Denver!H2+Huntersville!H2+Matthews!H2+'Rock Hill'!H2+Southpark!H2+FortMill!H2</f>
+        <f>Ballantyne!H2+Denver!H2+FortMill!H2+Huntersville!H2+Matthews!H2+'Rock Hill'!H2+Southpark!H2+Concord!H2+'Indian Trail'!H2+OtherDeNovo!H2</f>
         <v>0</v>
       </c>
       <c r="I2">
-        <f>Ballantyne!I2+Denver!I2+Huntersville!I2+Matthews!I2+'Rock Hill'!I2+Southpark!I2+FortMill!I2</f>
+        <f>Ballantyne!I2+Denver!I2+FortMill!I2+Huntersville!I2+Matthews!I2+'Rock Hill'!I2+Southpark!I2+Concord!I2+'Indian Trail'!I2+OtherDeNovo!I2</f>
         <v>0</v>
       </c>
       <c r="J2">
-        <f>Ballantyne!J2+Denver!J2+Huntersville!J2+Matthews!J2+'Rock Hill'!J2+Southpark!J2+FortMill!J2</f>
+        <f>Ballantyne!J2+Denver!J2+FortMill!J2+Huntersville!J2+Matthews!J2+'Rock Hill'!J2+Southpark!J2+Concord!J2+'Indian Trail'!J2+OtherDeNovo!J2</f>
         <v>0</v>
       </c>
       <c r="K2">
-        <f>Ballantyne!K2+Denver!K2+Huntersville!K2+Matthews!K2+'Rock Hill'!K2+Southpark!K2+FortMill!K2</f>
+        <f>Ballantyne!K2+Denver!K2+FortMill!K2+Huntersville!K2+Matthews!K2+'Rock Hill'!K2+Southpark!K2+Concord!K2+'Indian Trail'!K2+OtherDeNovo!K2</f>
         <v>0</v>
       </c>
       <c r="L2">
-        <f>Ballantyne!L2+Denver!L2+Huntersville!L2+Matthews!L2+'Rock Hill'!L2+Southpark!L2+FortMill!L2</f>
+        <f>Ballantyne!L2+Denver!L2+FortMill!L2+Huntersville!L2+Matthews!L2+'Rock Hill'!L2+Southpark!L2+Concord!L2+'Indian Trail'!L2+OtherDeNovo!L2</f>
         <v>0</v>
       </c>
       <c r="M2">
-        <f>Ballantyne!M2+Denver!M2+Huntersville!M2+Matthews!M2+'Rock Hill'!M2+Southpark!M2+FortMill!M2</f>
+        <f>Ballantyne!M2+Denver!M2+FortMill!M2+Huntersville!M2+Matthews!M2+'Rock Hill'!M2+Southpark!M2+Concord!M2+'Indian Trail'!M2+OtherDeNovo!M2</f>
         <v>0</v>
       </c>
       <c r="N2">
-        <f>Ballantyne!N2+Denver!N2+Huntersville!N2+Matthews!N2+'Rock Hill'!N2+Southpark!N2+FortMill!N2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+        <f>Ballantyne!N2+Denver!N2+FortMill!N2+Huntersville!N2+Matthews!N2+'Rock Hill'!N2+Southpark!N2+Concord!N2+'Indian Trail'!N2+OtherDeNovo!N2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -596,55 +605,55 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <f>Ballantyne!C3+Denver!C3+Huntersville!C3+Matthews!C3+'Rock Hill'!C3+Southpark!C3+FortMill!C3</f>
+        <f>Ballantyne!C3+Denver!C3+FortMill!C3+Huntersville!C3+Matthews!C3+'Rock Hill'!C3+Southpark!C3+Concord!C3+'Indian Trail'!C3+OtherDeNovo!C3</f>
         <v>0</v>
       </c>
       <c r="D3">
-        <f>Ballantyne!D3+Denver!D3+Huntersville!D3+Matthews!D3+'Rock Hill'!D3+Southpark!D3+FortMill!D3</f>
+        <f>Ballantyne!D3+Denver!D3+FortMill!D3+Huntersville!D3+Matthews!D3+'Rock Hill'!D3+Southpark!D3+Concord!D3+'Indian Trail'!D3+OtherDeNovo!D3</f>
         <v>0</v>
       </c>
       <c r="E3">
-        <f>Ballantyne!E3+Denver!E3+Huntersville!E3+Matthews!E3+'Rock Hill'!E3+Southpark!E3+FortMill!E3</f>
+        <f>Ballantyne!E3+Denver!E3+FortMill!E3+Huntersville!E3+Matthews!E3+'Rock Hill'!E3+Southpark!E3+Concord!E3+'Indian Trail'!E3+OtherDeNovo!E3</f>
         <v>0</v>
       </c>
       <c r="F3">
-        <f>Ballantyne!F3+Denver!F3+Huntersville!F3+Matthews!F3+'Rock Hill'!F3+Southpark!F3+FortMill!F3</f>
+        <f>Ballantyne!F3+Denver!F3+FortMill!F3+Huntersville!F3+Matthews!F3+'Rock Hill'!F3+Southpark!F3+Concord!F3+'Indian Trail'!F3+OtherDeNovo!F3</f>
         <v>0</v>
       </c>
       <c r="G3">
-        <f>Ballantyne!G3+Denver!G3+Huntersville!G3+Matthews!G3+'Rock Hill'!G3+Southpark!G3+FortMill!G3</f>
+        <f>Ballantyne!G3+Denver!G3+FortMill!G3+Huntersville!G3+Matthews!G3+'Rock Hill'!G3+Southpark!G3+Concord!G3+'Indian Trail'!G3+OtherDeNovo!G3</f>
         <v>0</v>
       </c>
       <c r="H3">
-        <f>Ballantyne!H3+Denver!H3+Huntersville!H3+Matthews!H3+'Rock Hill'!H3+Southpark!H3+FortMill!H3</f>
+        <f>Ballantyne!H3+Denver!H3+FortMill!H3+Huntersville!H3+Matthews!H3+'Rock Hill'!H3+Southpark!H3+Concord!H3+'Indian Trail'!H3+OtherDeNovo!H3</f>
         <v>0</v>
       </c>
       <c r="I3">
-        <f>Ballantyne!I3+Denver!I3+Huntersville!I3+Matthews!I3+'Rock Hill'!I3+Southpark!I3+FortMill!I3</f>
+        <f>Ballantyne!I3+Denver!I3+FortMill!I3+Huntersville!I3+Matthews!I3+'Rock Hill'!I3+Southpark!I3+Concord!I3+'Indian Trail'!I3+OtherDeNovo!I3</f>
         <v>0</v>
       </c>
       <c r="J3">
-        <f>Ballantyne!J3+Denver!J3+Huntersville!J3+Matthews!J3+'Rock Hill'!J3+Southpark!J3+FortMill!J3</f>
+        <f>Ballantyne!J3+Denver!J3+FortMill!J3+Huntersville!J3+Matthews!J3+'Rock Hill'!J3+Southpark!J3+Concord!J3+'Indian Trail'!J3+OtherDeNovo!J3</f>
         <v>0</v>
       </c>
       <c r="K3">
-        <f>Ballantyne!K3+Denver!K3+Huntersville!K3+Matthews!K3+'Rock Hill'!K3+Southpark!K3+FortMill!K3</f>
+        <f>Ballantyne!K3+Denver!K3+FortMill!K3+Huntersville!K3+Matthews!K3+'Rock Hill'!K3+Southpark!K3+Concord!K3+'Indian Trail'!K3+OtherDeNovo!K3</f>
         <v>0</v>
       </c>
       <c r="L3">
-        <f>Ballantyne!L3+Denver!L3+Huntersville!L3+Matthews!L3+'Rock Hill'!L3+Southpark!L3+FortMill!L3</f>
+        <f>Ballantyne!L3+Denver!L3+FortMill!L3+Huntersville!L3+Matthews!L3+'Rock Hill'!L3+Southpark!L3+Concord!L3+'Indian Trail'!L3+OtherDeNovo!L3</f>
         <v>0</v>
       </c>
       <c r="M3">
-        <f>Ballantyne!M3+Denver!M3+Huntersville!M3+Matthews!M3+'Rock Hill'!M3+Southpark!M3+FortMill!M3</f>
+        <f>Ballantyne!M3+Denver!M3+FortMill!M3+Huntersville!M3+Matthews!M3+'Rock Hill'!M3+Southpark!M3+Concord!M3+'Indian Trail'!M3+OtherDeNovo!M3</f>
         <v>0</v>
       </c>
       <c r="N3">
-        <f>Ballantyne!N3+Denver!N3+Huntersville!N3+Matthews!N3+'Rock Hill'!N3+Southpark!N3+FortMill!N3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+        <f>Ballantyne!N3+Denver!N3+FortMill!N3+Huntersville!N3+Matthews!N3+'Rock Hill'!N3+Southpark!N3+Concord!N3+'Indian Trail'!N3+OtherDeNovo!N3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -652,55 +661,55 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <f>Ballantyne!C4+Denver!C4+Huntersville!C4+Matthews!C4+'Rock Hill'!C4+Southpark!C4+FortMill!C4</f>
+        <f>Ballantyne!C4+Denver!C4+FortMill!C4+Huntersville!C4+Matthews!C4+'Rock Hill'!C4+Southpark!C4+Concord!C4+'Indian Trail'!C4+OtherDeNovo!C4</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f>Ballantyne!D4+Denver!D4+Huntersville!D4+Matthews!D4+'Rock Hill'!D4+Southpark!D4+FortMill!D4</f>
+        <f>Ballantyne!D4+Denver!D4+FortMill!D4+Huntersville!D4+Matthews!D4+'Rock Hill'!D4+Southpark!D4+Concord!D4+'Indian Trail'!D4+OtherDeNovo!D4</f>
         <v>0</v>
       </c>
       <c r="E4">
-        <f>Ballantyne!E4+Denver!E4+Huntersville!E4+Matthews!E4+'Rock Hill'!E4+Southpark!E4+FortMill!E4</f>
+        <f>Ballantyne!E4+Denver!E4+FortMill!E4+Huntersville!E4+Matthews!E4+'Rock Hill'!E4+Southpark!E4+Concord!E4+'Indian Trail'!E4+OtherDeNovo!E4</f>
         <v>0</v>
       </c>
       <c r="F4">
-        <f>Ballantyne!F4+Denver!F4+Huntersville!F4+Matthews!F4+'Rock Hill'!F4+Southpark!F4+FortMill!F4</f>
+        <f>Ballantyne!F4+Denver!F4+FortMill!F4+Huntersville!F4+Matthews!F4+'Rock Hill'!F4+Southpark!F4+Concord!F4+'Indian Trail'!F4+OtherDeNovo!F4</f>
         <v>0</v>
       </c>
       <c r="G4">
-        <f>Ballantyne!G4+Denver!G4+Huntersville!G4+Matthews!G4+'Rock Hill'!G4+Southpark!G4+FortMill!G4</f>
+        <f>Ballantyne!G4+Denver!G4+FortMill!G4+Huntersville!G4+Matthews!G4+'Rock Hill'!G4+Southpark!G4+Concord!G4+'Indian Trail'!G4+OtherDeNovo!G4</f>
         <v>0</v>
       </c>
       <c r="H4">
-        <f>Ballantyne!H4+Denver!H4+Huntersville!H4+Matthews!H4+'Rock Hill'!H4+Southpark!H4+FortMill!H4</f>
+        <f>Ballantyne!H4+Denver!H4+FortMill!H4+Huntersville!H4+Matthews!H4+'Rock Hill'!H4+Southpark!H4+Concord!H4+'Indian Trail'!H4+OtherDeNovo!H4</f>
         <v>0</v>
       </c>
       <c r="I4">
-        <f>Ballantyne!I4+Denver!I4+Huntersville!I4+Matthews!I4+'Rock Hill'!I4+Southpark!I4+FortMill!I4</f>
+        <f>Ballantyne!I4+Denver!I4+FortMill!I4+Huntersville!I4+Matthews!I4+'Rock Hill'!I4+Southpark!I4+Concord!I4+'Indian Trail'!I4+OtherDeNovo!I4</f>
         <v>0</v>
       </c>
       <c r="J4">
-        <f>Ballantyne!J4+Denver!J4+Huntersville!J4+Matthews!J4+'Rock Hill'!J4+Southpark!J4+FortMill!J4</f>
+        <f>Ballantyne!J4+Denver!J4+FortMill!J4+Huntersville!J4+Matthews!J4+'Rock Hill'!J4+Southpark!J4+Concord!J4+'Indian Trail'!J4+OtherDeNovo!J4</f>
         <v>0</v>
       </c>
       <c r="K4">
-        <f>Ballantyne!K4+Denver!K4+Huntersville!K4+Matthews!K4+'Rock Hill'!K4+Southpark!K4+FortMill!K4</f>
+        <f>Ballantyne!K4+Denver!K4+FortMill!K4+Huntersville!K4+Matthews!K4+'Rock Hill'!K4+Southpark!K4+Concord!K4+'Indian Trail'!K4+OtherDeNovo!K4</f>
         <v>0</v>
       </c>
       <c r="L4">
-        <f>Ballantyne!L4+Denver!L4+Huntersville!L4+Matthews!L4+'Rock Hill'!L4+Southpark!L4+FortMill!L4</f>
+        <f>Ballantyne!L4+Denver!L4+FortMill!L4+Huntersville!L4+Matthews!L4+'Rock Hill'!L4+Southpark!L4+Concord!L4+'Indian Trail'!L4+OtherDeNovo!L4</f>
         <v>0</v>
       </c>
       <c r="M4">
-        <f>Ballantyne!M4+Denver!M4+Huntersville!M4+Matthews!M4+'Rock Hill'!M4+Southpark!M4+FortMill!M4</f>
+        <f>Ballantyne!M4+Denver!M4+FortMill!M4+Huntersville!M4+Matthews!M4+'Rock Hill'!M4+Southpark!M4+Concord!M4+'Indian Trail'!M4+OtherDeNovo!M4</f>
         <v>0</v>
       </c>
       <c r="N4">
-        <f>Ballantyne!N4+Denver!N4+Huntersville!N4+Matthews!N4+'Rock Hill'!N4+Southpark!N4+FortMill!N4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+        <f>Ballantyne!N4+Denver!N4+FortMill!N4+Huntersville!N4+Matthews!N4+'Rock Hill'!N4+Southpark!N4+Concord!N4+'Indian Trail'!N4+OtherDeNovo!N4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -708,55 +717,55 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <f>Ballantyne!C5+Denver!C5+Huntersville!C5+Matthews!C5+'Rock Hill'!C5+Southpark!C5+FortMill!C5</f>
+        <f>Ballantyne!C5+Denver!C5+FortMill!C5+Huntersville!C5+Matthews!C5+'Rock Hill'!C5+Southpark!C5+Concord!C5+'Indian Trail'!C5+OtherDeNovo!C5</f>
         <v>0</v>
       </c>
       <c r="D5">
-        <f>Ballantyne!D5+Denver!D5+Huntersville!D5+Matthews!D5+'Rock Hill'!D5+Southpark!D5+FortMill!D5</f>
+        <f>Ballantyne!D5+Denver!D5+FortMill!D5+Huntersville!D5+Matthews!D5+'Rock Hill'!D5+Southpark!D5+Concord!D5+'Indian Trail'!D5+OtherDeNovo!D5</f>
         <v>0</v>
       </c>
       <c r="E5">
-        <f>Ballantyne!E5+Denver!E5+Huntersville!E5+Matthews!E5+'Rock Hill'!E5+Southpark!E5+FortMill!E5</f>
+        <f>Ballantyne!E5+Denver!E5+FortMill!E5+Huntersville!E5+Matthews!E5+'Rock Hill'!E5+Southpark!E5+Concord!E5+'Indian Trail'!E5+OtherDeNovo!E5</f>
         <v>0</v>
       </c>
       <c r="F5">
-        <f>Ballantyne!F5+Denver!F5+Huntersville!F5+Matthews!F5+'Rock Hill'!F5+Southpark!F5+FortMill!F5</f>
+        <f>Ballantyne!F5+Denver!F5+FortMill!F5+Huntersville!F5+Matthews!F5+'Rock Hill'!F5+Southpark!F5+Concord!F5+'Indian Trail'!F5+OtherDeNovo!F5</f>
         <v>0</v>
       </c>
       <c r="G5">
-        <f>Ballantyne!G5+Denver!G5+Huntersville!G5+Matthews!G5+'Rock Hill'!G5+Southpark!G5+FortMill!G5</f>
+        <f>Ballantyne!G5+Denver!G5+FortMill!G5+Huntersville!G5+Matthews!G5+'Rock Hill'!G5+Southpark!G5+Concord!G5+'Indian Trail'!G5+OtherDeNovo!G5</f>
         <v>0</v>
       </c>
       <c r="H5">
-        <f>Ballantyne!H5+Denver!H5+Huntersville!H5+Matthews!H5+'Rock Hill'!H5+Southpark!H5+FortMill!H5</f>
+        <f>Ballantyne!H5+Denver!H5+FortMill!H5+Huntersville!H5+Matthews!H5+'Rock Hill'!H5+Southpark!H5+Concord!H5+'Indian Trail'!H5+OtherDeNovo!H5</f>
         <v>0</v>
       </c>
       <c r="I5">
-        <f>Ballantyne!I5+Denver!I5+Huntersville!I5+Matthews!I5+'Rock Hill'!I5+Southpark!I5+FortMill!I5</f>
+        <f>Ballantyne!I5+Denver!I5+FortMill!I5+Huntersville!I5+Matthews!I5+'Rock Hill'!I5+Southpark!I5+Concord!I5+'Indian Trail'!I5+OtherDeNovo!I5</f>
         <v>0</v>
       </c>
       <c r="J5">
-        <f>Ballantyne!J5+Denver!J5+Huntersville!J5+Matthews!J5+'Rock Hill'!J5+Southpark!J5+FortMill!J5</f>
+        <f>Ballantyne!J5+Denver!J5+FortMill!J5+Huntersville!J5+Matthews!J5+'Rock Hill'!J5+Southpark!J5+Concord!J5+'Indian Trail'!J5+OtherDeNovo!J5</f>
         <v>0</v>
       </c>
       <c r="K5">
-        <f>Ballantyne!K5+Denver!K5+Huntersville!K5+Matthews!K5+'Rock Hill'!K5+Southpark!K5+FortMill!K5</f>
+        <f>Ballantyne!K5+Denver!K5+FortMill!K5+Huntersville!K5+Matthews!K5+'Rock Hill'!K5+Southpark!K5+Concord!K5+'Indian Trail'!K5+OtherDeNovo!K5</f>
         <v>0</v>
       </c>
       <c r="L5">
-        <f>Ballantyne!L5+Denver!L5+Huntersville!L5+Matthews!L5+'Rock Hill'!L5+Southpark!L5+FortMill!L5</f>
+        <f>Ballantyne!L5+Denver!L5+FortMill!L5+Huntersville!L5+Matthews!L5+'Rock Hill'!L5+Southpark!L5+Concord!L5+'Indian Trail'!L5+OtherDeNovo!L5</f>
         <v>0</v>
       </c>
       <c r="M5">
-        <f>Ballantyne!M5+Denver!M5+Huntersville!M5+Matthews!M5+'Rock Hill'!M5+Southpark!M5+FortMill!M5</f>
+        <f>Ballantyne!M5+Denver!M5+FortMill!M5+Huntersville!M5+Matthews!M5+'Rock Hill'!M5+Southpark!M5+Concord!M5+'Indian Trail'!M5+OtherDeNovo!M5</f>
         <v>0</v>
       </c>
       <c r="N5">
-        <f>Ballantyne!N5+Denver!N5+Huntersville!N5+Matthews!N5+'Rock Hill'!N5+Southpark!N5+FortMill!N5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <f>Ballantyne!N5+Denver!N5+FortMill!N5+Huntersville!N5+Matthews!N5+'Rock Hill'!N5+Southpark!N5+Concord!N5+'Indian Trail'!N5+OtherDeNovo!N5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -764,55 +773,55 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <f>Ballantyne!C6+Denver!C6+Huntersville!C6+Matthews!C6+'Rock Hill'!C6+Southpark!C6+FortMill!C6</f>
+        <f>Ballantyne!C6+Denver!C6+FortMill!C6+Huntersville!C6+Matthews!C6+'Rock Hill'!C6+Southpark!C6+Concord!C6+'Indian Trail'!C6+OtherDeNovo!C6</f>
         <v>0</v>
       </c>
       <c r="D6">
-        <f>Ballantyne!D6+Denver!D6+Huntersville!D6+Matthews!D6+'Rock Hill'!D6+Southpark!D6+FortMill!D6</f>
+        <f>Ballantyne!D6+Denver!D6+FortMill!D6+Huntersville!D6+Matthews!D6+'Rock Hill'!D6+Southpark!D6+Concord!D6+'Indian Trail'!D6+OtherDeNovo!D6</f>
         <v>0</v>
       </c>
       <c r="E6">
-        <f>Ballantyne!E6+Denver!E6+Huntersville!E6+Matthews!E6+'Rock Hill'!E6+Southpark!E6+FortMill!E6</f>
+        <f>Ballantyne!E6+Denver!E6+FortMill!E6+Huntersville!E6+Matthews!E6+'Rock Hill'!E6+Southpark!E6+Concord!E6+'Indian Trail'!E6+OtherDeNovo!E6</f>
         <v>0</v>
       </c>
       <c r="F6">
-        <f>Ballantyne!F6+Denver!F6+Huntersville!F6+Matthews!F6+'Rock Hill'!F6+Southpark!F6+FortMill!F6</f>
+        <f>Ballantyne!F6+Denver!F6+FortMill!F6+Huntersville!F6+Matthews!F6+'Rock Hill'!F6+Southpark!F6+Concord!F6+'Indian Trail'!F6+OtherDeNovo!F6</f>
         <v>0</v>
       </c>
       <c r="G6">
-        <f>Ballantyne!G6+Denver!G6+Huntersville!G6+Matthews!G6+'Rock Hill'!G6+Southpark!G6+FortMill!G6</f>
+        <f>Ballantyne!G6+Denver!G6+FortMill!G6+Huntersville!G6+Matthews!G6+'Rock Hill'!G6+Southpark!G6+Concord!G6+'Indian Trail'!G6+OtherDeNovo!G6</f>
         <v>0</v>
       </c>
       <c r="H6">
-        <f>Ballantyne!H6+Denver!H6+Huntersville!H6+Matthews!H6+'Rock Hill'!H6+Southpark!H6+FortMill!H6</f>
+        <f>Ballantyne!H6+Denver!H6+FortMill!H6+Huntersville!H6+Matthews!H6+'Rock Hill'!H6+Southpark!H6+Concord!H6+'Indian Trail'!H6+OtherDeNovo!H6</f>
         <v>0</v>
       </c>
       <c r="I6">
-        <f>Ballantyne!I6+Denver!I6+Huntersville!I6+Matthews!I6+'Rock Hill'!I6+Southpark!I6+FortMill!I6</f>
+        <f>Ballantyne!I6+Denver!I6+FortMill!I6+Huntersville!I6+Matthews!I6+'Rock Hill'!I6+Southpark!I6+Concord!I6+'Indian Trail'!I6+OtherDeNovo!I6</f>
         <v>0</v>
       </c>
       <c r="J6">
-        <f>Ballantyne!J6+Denver!J6+Huntersville!J6+Matthews!J6+'Rock Hill'!J6+Southpark!J6+FortMill!J6</f>
+        <f>Ballantyne!J6+Denver!J6+FortMill!J6+Huntersville!J6+Matthews!J6+'Rock Hill'!J6+Southpark!J6+Concord!J6+'Indian Trail'!J6+OtherDeNovo!J6</f>
         <v>0</v>
       </c>
       <c r="K6">
-        <f>Ballantyne!K6+Denver!K6+Huntersville!K6+Matthews!K6+'Rock Hill'!K6+Southpark!K6+FortMill!K6</f>
+        <f>Ballantyne!K6+Denver!K6+FortMill!K6+Huntersville!K6+Matthews!K6+'Rock Hill'!K6+Southpark!K6+Concord!K6+'Indian Trail'!K6+OtherDeNovo!K6</f>
         <v>0</v>
       </c>
       <c r="L6">
-        <f>Ballantyne!L6+Denver!L6+Huntersville!L6+Matthews!L6+'Rock Hill'!L6+Southpark!L6+FortMill!L6</f>
+        <f>Ballantyne!L6+Denver!L6+FortMill!L6+Huntersville!L6+Matthews!L6+'Rock Hill'!L6+Southpark!L6+Concord!L6+'Indian Trail'!L6+OtherDeNovo!L6</f>
         <v>0</v>
       </c>
       <c r="M6">
-        <f>Ballantyne!M6+Denver!M6+Huntersville!M6+Matthews!M6+'Rock Hill'!M6+Southpark!M6+FortMill!M6</f>
+        <f>Ballantyne!M6+Denver!M6+FortMill!M6+Huntersville!M6+Matthews!M6+'Rock Hill'!M6+Southpark!M6+Concord!M6+'Indian Trail'!M6+OtherDeNovo!M6</f>
         <v>0</v>
       </c>
       <c r="N6">
-        <f>Ballantyne!N6+Denver!N6+Huntersville!N6+Matthews!N6+'Rock Hill'!N6+Southpark!N6+FortMill!N6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+        <f>Ballantyne!N6+Denver!N6+FortMill!N6+Huntersville!N6+Matthews!N6+'Rock Hill'!N6+Southpark!N6+Concord!N6+'Indian Trail'!N6+OtherDeNovo!N6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -820,55 +829,55 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <f>Ballantyne!C7+Denver!C7+Huntersville!C7+Matthews!C7+'Rock Hill'!C7+Southpark!C7+FortMill!C7</f>
+        <f>Ballantyne!C7+Denver!C7+FortMill!C7+Huntersville!C7+Matthews!C7+'Rock Hill'!C7+Southpark!C7+Concord!C7+'Indian Trail'!C7+OtherDeNovo!C7</f>
         <v>0</v>
       </c>
       <c r="D7">
-        <f>Ballantyne!D7+Denver!D7+Huntersville!D7+Matthews!D7+'Rock Hill'!D7+Southpark!D7+FortMill!D7</f>
+        <f>Ballantyne!D7+Denver!D7+FortMill!D7+Huntersville!D7+Matthews!D7+'Rock Hill'!D7+Southpark!D7+Concord!D7+'Indian Trail'!D7+OtherDeNovo!D7</f>
         <v>0</v>
       </c>
       <c r="E7">
-        <f>Ballantyne!E7+Denver!E7+Huntersville!E7+Matthews!E7+'Rock Hill'!E7+Southpark!E7+FortMill!E7</f>
+        <f>Ballantyne!E7+Denver!E7+FortMill!E7+Huntersville!E7+Matthews!E7+'Rock Hill'!E7+Southpark!E7+Concord!E7+'Indian Trail'!E7+OtherDeNovo!E7</f>
         <v>0</v>
       </c>
       <c r="F7">
-        <f>Ballantyne!F7+Denver!F7+Huntersville!F7+Matthews!F7+'Rock Hill'!F7+Southpark!F7+FortMill!F7</f>
+        <f>Ballantyne!F7+Denver!F7+FortMill!F7+Huntersville!F7+Matthews!F7+'Rock Hill'!F7+Southpark!F7+Concord!F7+'Indian Trail'!F7+OtherDeNovo!F7</f>
         <v>0</v>
       </c>
       <c r="G7">
-        <f>Ballantyne!G7+Denver!G7+Huntersville!G7+Matthews!G7+'Rock Hill'!G7+Southpark!G7+FortMill!G7</f>
+        <f>Ballantyne!G7+Denver!G7+FortMill!G7+Huntersville!G7+Matthews!G7+'Rock Hill'!G7+Southpark!G7+Concord!G7+'Indian Trail'!G7+OtherDeNovo!G7</f>
         <v>0</v>
       </c>
       <c r="H7">
-        <f>Ballantyne!H7+Denver!H7+Huntersville!H7+Matthews!H7+'Rock Hill'!H7+Southpark!H7+FortMill!H7</f>
+        <f>Ballantyne!H7+Denver!H7+FortMill!H7+Huntersville!H7+Matthews!H7+'Rock Hill'!H7+Southpark!H7+Concord!H7+'Indian Trail'!H7+OtherDeNovo!H7</f>
         <v>0</v>
       </c>
       <c r="I7">
-        <f>Ballantyne!I7+Denver!I7+Huntersville!I7+Matthews!I7+'Rock Hill'!I7+Southpark!I7+FortMill!I7</f>
+        <f>Ballantyne!I7+Denver!I7+FortMill!I7+Huntersville!I7+Matthews!I7+'Rock Hill'!I7+Southpark!I7+Concord!I7+'Indian Trail'!I7+OtherDeNovo!I7</f>
         <v>0</v>
       </c>
       <c r="J7">
-        <f>Ballantyne!J7+Denver!J7+Huntersville!J7+Matthews!J7+'Rock Hill'!J7+Southpark!J7+FortMill!J7</f>
+        <f>Ballantyne!J7+Denver!J7+FortMill!J7+Huntersville!J7+Matthews!J7+'Rock Hill'!J7+Southpark!J7+Concord!J7+'Indian Trail'!J7+OtherDeNovo!J7</f>
         <v>0</v>
       </c>
       <c r="K7">
-        <f>Ballantyne!K7+Denver!K7+Huntersville!K7+Matthews!K7+'Rock Hill'!K7+Southpark!K7+FortMill!K7</f>
+        <f>Ballantyne!K7+Denver!K7+FortMill!K7+Huntersville!K7+Matthews!K7+'Rock Hill'!K7+Southpark!K7+Concord!K7+'Indian Trail'!K7+OtherDeNovo!K7</f>
         <v>0</v>
       </c>
       <c r="L7">
-        <f>Ballantyne!L7+Denver!L7+Huntersville!L7+Matthews!L7+'Rock Hill'!L7+Southpark!L7+FortMill!L7</f>
+        <f>Ballantyne!L7+Denver!L7+FortMill!L7+Huntersville!L7+Matthews!L7+'Rock Hill'!L7+Southpark!L7+Concord!L7+'Indian Trail'!L7+OtherDeNovo!L7</f>
         <v>0</v>
       </c>
       <c r="M7">
-        <f>Ballantyne!M7+Denver!M7+Huntersville!M7+Matthews!M7+'Rock Hill'!M7+Southpark!M7+FortMill!M7</f>
+        <f>Ballantyne!M7+Denver!M7+FortMill!M7+Huntersville!M7+Matthews!M7+'Rock Hill'!M7+Southpark!M7+Concord!M7+'Indian Trail'!M7+OtherDeNovo!M7</f>
         <v>0</v>
       </c>
       <c r="N7">
-        <f>Ballantyne!N7+Denver!N7+Huntersville!N7+Matthews!N7+'Rock Hill'!N7+Southpark!N7+FortMill!N7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+        <f>Ballantyne!N7+Denver!N7+FortMill!N7+Huntersville!N7+Matthews!N7+'Rock Hill'!N7+Southpark!N7+Concord!N7+'Indian Trail'!N7+OtherDeNovo!N7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -876,55 +885,55 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <f>Ballantyne!C8+Denver!C8+Huntersville!C8+Matthews!C8+'Rock Hill'!C8+Southpark!C8+FortMill!C8</f>
+        <f>Ballantyne!C8+Denver!C8+FortMill!C8+Huntersville!C8+Matthews!C8+'Rock Hill'!C8+Southpark!C8+Concord!C8+'Indian Trail'!C8+OtherDeNovo!C8</f>
         <v>0</v>
       </c>
       <c r="D8">
-        <f>Ballantyne!D8+Denver!D8+Huntersville!D8+Matthews!D8+'Rock Hill'!D8+Southpark!D8+FortMill!D8</f>
+        <f>Ballantyne!D8+Denver!D8+FortMill!D8+Huntersville!D8+Matthews!D8+'Rock Hill'!D8+Southpark!D8+Concord!D8+'Indian Trail'!D8+OtherDeNovo!D8</f>
         <v>0</v>
       </c>
       <c r="E8">
-        <f>Ballantyne!E8+Denver!E8+Huntersville!E8+Matthews!E8+'Rock Hill'!E8+Southpark!E8+FortMill!E8</f>
+        <f>Ballantyne!E8+Denver!E8+FortMill!E8+Huntersville!E8+Matthews!E8+'Rock Hill'!E8+Southpark!E8+Concord!E8+'Indian Trail'!E8+OtherDeNovo!E8</f>
         <v>0</v>
       </c>
       <c r="F8">
-        <f>Ballantyne!F8+Denver!F8+Huntersville!F8+Matthews!F8+'Rock Hill'!F8+Southpark!F8+FortMill!F8</f>
+        <f>Ballantyne!F8+Denver!F8+FortMill!F8+Huntersville!F8+Matthews!F8+'Rock Hill'!F8+Southpark!F8+Concord!F8+'Indian Trail'!F8+OtherDeNovo!F8</f>
         <v>0</v>
       </c>
       <c r="G8">
-        <f>Ballantyne!G8+Denver!G8+Huntersville!G8+Matthews!G8+'Rock Hill'!G8+Southpark!G8+FortMill!G8</f>
+        <f>Ballantyne!G8+Denver!G8+FortMill!G8+Huntersville!G8+Matthews!G8+'Rock Hill'!G8+Southpark!G8+Concord!G8+'Indian Trail'!G8+OtherDeNovo!G8</f>
         <v>0</v>
       </c>
       <c r="H8">
-        <f>Ballantyne!H8+Denver!H8+Huntersville!H8+Matthews!H8+'Rock Hill'!H8+Southpark!H8+FortMill!H8</f>
+        <f>Ballantyne!H8+Denver!H8+FortMill!H8+Huntersville!H8+Matthews!H8+'Rock Hill'!H8+Southpark!H8+Concord!H8+'Indian Trail'!H8+OtherDeNovo!H8</f>
         <v>0</v>
       </c>
       <c r="I8">
-        <f>Ballantyne!I8+Denver!I8+Huntersville!I8+Matthews!I8+'Rock Hill'!I8+Southpark!I8+FortMill!I8</f>
+        <f>Ballantyne!I8+Denver!I8+FortMill!I8+Huntersville!I8+Matthews!I8+'Rock Hill'!I8+Southpark!I8+Concord!I8+'Indian Trail'!I8+OtherDeNovo!I8</f>
         <v>0</v>
       </c>
       <c r="J8">
-        <f>Ballantyne!J8+Denver!J8+Huntersville!J8+Matthews!J8+'Rock Hill'!J8+Southpark!J8+FortMill!J8</f>
+        <f>Ballantyne!J8+Denver!J8+FortMill!J8+Huntersville!J8+Matthews!J8+'Rock Hill'!J8+Southpark!J8+Concord!J8+'Indian Trail'!J8+OtherDeNovo!J8</f>
         <v>0</v>
       </c>
       <c r="K8">
-        <f>Ballantyne!K8+Denver!K8+Huntersville!K8+Matthews!K8+'Rock Hill'!K8+Southpark!K8+FortMill!K8</f>
+        <f>Ballantyne!K8+Denver!K8+FortMill!K8+Huntersville!K8+Matthews!K8+'Rock Hill'!K8+Southpark!K8+Concord!K8+'Indian Trail'!K8+OtherDeNovo!K8</f>
         <v>0</v>
       </c>
       <c r="L8">
-        <f>Ballantyne!L8+Denver!L8+Huntersville!L8+Matthews!L8+'Rock Hill'!L8+Southpark!L8+FortMill!L8</f>
+        <f>Ballantyne!L8+Denver!L8+FortMill!L8+Huntersville!L8+Matthews!L8+'Rock Hill'!L8+Southpark!L8+Concord!L8+'Indian Trail'!L8+OtherDeNovo!L8</f>
         <v>0</v>
       </c>
       <c r="M8">
-        <f>Ballantyne!M8+Denver!M8+Huntersville!M8+Matthews!M8+'Rock Hill'!M8+Southpark!M8+FortMill!M8</f>
+        <f>Ballantyne!M8+Denver!M8+FortMill!M8+Huntersville!M8+Matthews!M8+'Rock Hill'!M8+Southpark!M8+Concord!M8+'Indian Trail'!M8+OtherDeNovo!M8</f>
         <v>0</v>
       </c>
       <c r="N8">
-        <f>Ballantyne!N8+Denver!N8+Huntersville!N8+Matthews!N8+'Rock Hill'!N8+Southpark!N8+FortMill!N8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+        <f>Ballantyne!N8+Denver!N8+FortMill!N8+Huntersville!N8+Matthews!N8+'Rock Hill'!N8+Southpark!N8+Concord!N8+'Indian Trail'!N8+OtherDeNovo!N8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -932,55 +941,55 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <f>Ballantyne!C9+Denver!C9+Huntersville!C9+Matthews!C9+'Rock Hill'!C9+Southpark!C9+FortMill!C9</f>
+        <f>Ballantyne!C9+Denver!C9+FortMill!C9+Huntersville!C9+Matthews!C9+'Rock Hill'!C9+Southpark!C9+Concord!C9+'Indian Trail'!C9+OtherDeNovo!C9</f>
         <v>0</v>
       </c>
       <c r="D9">
-        <f>Ballantyne!D9+Denver!D9+Huntersville!D9+Matthews!D9+'Rock Hill'!D9+Southpark!D9+FortMill!D9</f>
+        <f>Ballantyne!D9+Denver!D9+FortMill!D9+Huntersville!D9+Matthews!D9+'Rock Hill'!D9+Southpark!D9+Concord!D9+'Indian Trail'!D9+OtherDeNovo!D9</f>
         <v>0</v>
       </c>
       <c r="E9">
-        <f>Ballantyne!E9+Denver!E9+Huntersville!E9+Matthews!E9+'Rock Hill'!E9+Southpark!E9+FortMill!E9</f>
+        <f>Ballantyne!E9+Denver!E9+FortMill!E9+Huntersville!E9+Matthews!E9+'Rock Hill'!E9+Southpark!E9+Concord!E9+'Indian Trail'!E9+OtherDeNovo!E9</f>
         <v>0</v>
       </c>
       <c r="F9">
-        <f>Ballantyne!F9+Denver!F9+Huntersville!F9+Matthews!F9+'Rock Hill'!F9+Southpark!F9+FortMill!F9</f>
+        <f>Ballantyne!F9+Denver!F9+FortMill!F9+Huntersville!F9+Matthews!F9+'Rock Hill'!F9+Southpark!F9+Concord!F9+'Indian Trail'!F9+OtherDeNovo!F9</f>
         <v>0</v>
       </c>
       <c r="G9">
-        <f>Ballantyne!G9+Denver!G9+Huntersville!G9+Matthews!G9+'Rock Hill'!G9+Southpark!G9+FortMill!G9</f>
+        <f>Ballantyne!G9+Denver!G9+FortMill!G9+Huntersville!G9+Matthews!G9+'Rock Hill'!G9+Southpark!G9+Concord!G9+'Indian Trail'!G9+OtherDeNovo!G9</f>
         <v>0</v>
       </c>
       <c r="H9">
-        <f>Ballantyne!H9+Denver!H9+Huntersville!H9+Matthews!H9+'Rock Hill'!H9+Southpark!H9+FortMill!H9</f>
+        <f>Ballantyne!H9+Denver!H9+FortMill!H9+Huntersville!H9+Matthews!H9+'Rock Hill'!H9+Southpark!H9+Concord!H9+'Indian Trail'!H9+OtherDeNovo!H9</f>
         <v>0</v>
       </c>
       <c r="I9">
-        <f>Ballantyne!I9+Denver!I9+Huntersville!I9+Matthews!I9+'Rock Hill'!I9+Southpark!I9+FortMill!I9</f>
+        <f>Ballantyne!I9+Denver!I9+FortMill!I9+Huntersville!I9+Matthews!I9+'Rock Hill'!I9+Southpark!I9+Concord!I9+'Indian Trail'!I9+OtherDeNovo!I9</f>
         <v>0</v>
       </c>
       <c r="J9">
-        <f>Ballantyne!J9+Denver!J9+Huntersville!J9+Matthews!J9+'Rock Hill'!J9+Southpark!J9+FortMill!J9</f>
+        <f>Ballantyne!J9+Denver!J9+FortMill!J9+Huntersville!J9+Matthews!J9+'Rock Hill'!J9+Southpark!J9+Concord!J9+'Indian Trail'!J9+OtherDeNovo!J9</f>
         <v>0</v>
       </c>
       <c r="K9">
-        <f>Ballantyne!K9+Denver!K9+Huntersville!K9+Matthews!K9+'Rock Hill'!K9+Southpark!K9+FortMill!K9</f>
+        <f>Ballantyne!K9+Denver!K9+FortMill!K9+Huntersville!K9+Matthews!K9+'Rock Hill'!K9+Southpark!K9+Concord!K9+'Indian Trail'!K9+OtherDeNovo!K9</f>
         <v>0</v>
       </c>
       <c r="L9">
-        <f>Ballantyne!L9+Denver!L9+Huntersville!L9+Matthews!L9+'Rock Hill'!L9+Southpark!L9+FortMill!L9</f>
+        <f>Ballantyne!L9+Denver!L9+FortMill!L9+Huntersville!L9+Matthews!L9+'Rock Hill'!L9+Southpark!L9+Concord!L9+'Indian Trail'!L9+OtherDeNovo!L9</f>
         <v>0</v>
       </c>
       <c r="M9">
-        <f>Ballantyne!M9+Denver!M9+Huntersville!M9+Matthews!M9+'Rock Hill'!M9+Southpark!M9+FortMill!M9</f>
+        <f>Ballantyne!M9+Denver!M9+FortMill!M9+Huntersville!M9+Matthews!M9+'Rock Hill'!M9+Southpark!M9+Concord!M9+'Indian Trail'!M9+OtherDeNovo!M9</f>
         <v>0</v>
       </c>
       <c r="N9">
-        <f>Ballantyne!N9+Denver!N9+Huntersville!N9+Matthews!N9+'Rock Hill'!N9+Southpark!N9+FortMill!N9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+        <f>Ballantyne!N9+Denver!N9+FortMill!N9+Huntersville!N9+Matthews!N9+'Rock Hill'!N9+Southpark!N9+Concord!N9+'Indian Trail'!N9+OtherDeNovo!N9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -988,52 +997,534 @@
         <v>2</v>
       </c>
       <c r="C10">
-        <f>Ballantyne!C10+Denver!C10+Huntersville!C10+Matthews!C10+'Rock Hill'!C10+Southpark!C10+FortMill!C10</f>
+        <f>Ballantyne!C10+Denver!C10+FortMill!C10+Huntersville!C10+Matthews!C10+'Rock Hill'!C10+Southpark!C10+Concord!C10+'Indian Trail'!C10+OtherDeNovo!C10</f>
         <v>0</v>
       </c>
       <c r="D10">
-        <f>Ballantyne!D10+Denver!D10+Huntersville!D10+Matthews!D10+'Rock Hill'!D10+Southpark!D10+FortMill!D10</f>
+        <f>Ballantyne!D10+Denver!D10+FortMill!D10+Huntersville!D10+Matthews!D10+'Rock Hill'!D10+Southpark!D10+Concord!D10+'Indian Trail'!D10+OtherDeNovo!D10</f>
         <v>0</v>
       </c>
       <c r="E10">
-        <f>Ballantyne!E10+Denver!E10+Huntersville!E10+Matthews!E10+'Rock Hill'!E10+Southpark!E10+FortMill!E10</f>
+        <f>Ballantyne!E10+Denver!E10+FortMill!E10+Huntersville!E10+Matthews!E10+'Rock Hill'!E10+Southpark!E10+Concord!E10+'Indian Trail'!E10+OtherDeNovo!E10</f>
         <v>0</v>
       </c>
       <c r="F10">
-        <f>Ballantyne!F10+Denver!F10+Huntersville!F10+Matthews!F10+'Rock Hill'!F10+Southpark!F10+FortMill!F10</f>
+        <f>Ballantyne!F10+Denver!F10+FortMill!F10+Huntersville!F10+Matthews!F10+'Rock Hill'!F10+Southpark!F10+Concord!F10+'Indian Trail'!F10+OtherDeNovo!F10</f>
         <v>0</v>
       </c>
       <c r="G10">
-        <f>Ballantyne!G10+Denver!G10+Huntersville!G10+Matthews!G10+'Rock Hill'!G10+Southpark!G10+FortMill!G10</f>
+        <f>Ballantyne!G10+Denver!G10+FortMill!G10+Huntersville!G10+Matthews!G10+'Rock Hill'!G10+Southpark!G10+Concord!G10+'Indian Trail'!G10+OtherDeNovo!G10</f>
         <v>0</v>
       </c>
       <c r="H10">
-        <f>Ballantyne!H10+Denver!H10+Huntersville!H10+Matthews!H10+'Rock Hill'!H10+Southpark!H10+FortMill!H10</f>
+        <f>Ballantyne!H10+Denver!H10+FortMill!H10+Huntersville!H10+Matthews!H10+'Rock Hill'!H10+Southpark!H10+Concord!H10+'Indian Trail'!H10+OtherDeNovo!H10</f>
         <v>0</v>
       </c>
       <c r="I10">
-        <f>Ballantyne!I10+Denver!I10+Huntersville!I10+Matthews!I10+'Rock Hill'!I10+Southpark!I10+FortMill!I10</f>
+        <f>Ballantyne!I10+Denver!I10+FortMill!I10+Huntersville!I10+Matthews!I10+'Rock Hill'!I10+Southpark!I10+Concord!I10+'Indian Trail'!I10+OtherDeNovo!I10</f>
         <v>0</v>
       </c>
       <c r="J10">
-        <f>Ballantyne!J10+Denver!J10+Huntersville!J10+Matthews!J10+'Rock Hill'!J10+Southpark!J10+FortMill!J10</f>
+        <f>Ballantyne!J10+Denver!J10+FortMill!J10+Huntersville!J10+Matthews!J10+'Rock Hill'!J10+Southpark!J10+Concord!J10+'Indian Trail'!J10+OtherDeNovo!J10</f>
         <v>0</v>
       </c>
       <c r="K10">
-        <f>Ballantyne!K10+Denver!K10+Huntersville!K10+Matthews!K10+'Rock Hill'!K10+Southpark!K10+FortMill!K10</f>
+        <f>Ballantyne!K10+Denver!K10+FortMill!K10+Huntersville!K10+Matthews!K10+'Rock Hill'!K10+Southpark!K10+Concord!K10+'Indian Trail'!K10+OtherDeNovo!K10</f>
         <v>0</v>
       </c>
       <c r="L10">
-        <f>Ballantyne!L10+Denver!L10+Huntersville!L10+Matthews!L10+'Rock Hill'!L10+Southpark!L10+FortMill!L10</f>
+        <f>Ballantyne!L10+Denver!L10+FortMill!L10+Huntersville!L10+Matthews!L10+'Rock Hill'!L10+Southpark!L10+Concord!L10+'Indian Trail'!L10+OtherDeNovo!L10</f>
         <v>0</v>
       </c>
       <c r="M10">
-        <f>Ballantyne!M10+Denver!M10+Huntersville!M10+Matthews!M10+'Rock Hill'!M10+Southpark!M10+FortMill!M10</f>
+        <f>Ballantyne!M10+Denver!M10+FortMill!M10+Huntersville!M10+Matthews!M10+'Rock Hill'!M10+Southpark!M10+Concord!M10+'Indian Trail'!M10+OtherDeNovo!M10</f>
         <v>0</v>
       </c>
       <c r="N10">
-        <f>Ballantyne!N10+Denver!N10+Huntersville!N10+Matthews!N10+'Rock Hill'!N10+Southpark!N10+FortMill!N10</f>
-        <v>0</v>
+        <f>Ballantyne!N10+Denver!N10+FortMill!N10+Huntersville!N10+Matthews!N10+'Rock Hill'!N10+Southpark!N10+Concord!N10+'Indian Trail'!N10+OtherDeNovo!N10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <f>Ballantyne!C11+Denver!C11+FortMill!C11+Huntersville!C11+Matthews!C11+'Rock Hill'!C11+Southpark!C11+Concord!C11+'Indian Trail'!C11+OtherDeNovo!C11</f>
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f>Ballantyne!D11+Denver!D11+FortMill!D11+Huntersville!D11+Matthews!D11+'Rock Hill'!D11+Southpark!D11+Concord!D11+'Indian Trail'!D11+OtherDeNovo!D11</f>
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f>Ballantyne!E11+Denver!E11+FortMill!E11+Huntersville!E11+Matthews!E11+'Rock Hill'!E11+Southpark!E11+Concord!E11+'Indian Trail'!E11+OtherDeNovo!E11</f>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f>Ballantyne!F11+Denver!F11+FortMill!F11+Huntersville!F11+Matthews!F11+'Rock Hill'!F11+Southpark!F11+Concord!F11+'Indian Trail'!F11+OtherDeNovo!F11</f>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f>Ballantyne!G11+Denver!G11+FortMill!G11+Huntersville!G11+Matthews!G11+'Rock Hill'!G11+Southpark!G11+Concord!G11+'Indian Trail'!G11+OtherDeNovo!G11</f>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f>Ballantyne!H11+Denver!H11+FortMill!H11+Huntersville!H11+Matthews!H11+'Rock Hill'!H11+Southpark!H11+Concord!H11+'Indian Trail'!H11+OtherDeNovo!H11</f>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f>Ballantyne!I11+Denver!I11+FortMill!I11+Huntersville!I11+Matthews!I11+'Rock Hill'!I11+Southpark!I11+Concord!I11+'Indian Trail'!I11+OtherDeNovo!I11</f>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <f>Ballantyne!J11+Denver!J11+FortMill!J11+Huntersville!J11+Matthews!J11+'Rock Hill'!J11+Southpark!J11+Concord!J11+'Indian Trail'!J11+OtherDeNovo!J11</f>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <f>Ballantyne!K11+Denver!K11+FortMill!K11+Huntersville!K11+Matthews!K11+'Rock Hill'!K11+Southpark!K11+Concord!K11+'Indian Trail'!K11+OtherDeNovo!K11</f>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f>Ballantyne!L11+Denver!L11+FortMill!L11+Huntersville!L11+Matthews!L11+'Rock Hill'!L11+Southpark!L11+Concord!L11+'Indian Trail'!L11+OtherDeNovo!L11</f>
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <f>Ballantyne!M11+Denver!M11+FortMill!M11+Huntersville!M11+Matthews!M11+'Rock Hill'!M11+Southpark!M11+Concord!M11+'Indian Trail'!M11+OtherDeNovo!M11</f>
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <f>Ballantyne!N11+Denver!N11+FortMill!N11+Huntersville!N11+Matthews!N11+'Rock Hill'!N11+Southpark!N11+Concord!N11+'Indian Trail'!N11+OtherDeNovo!N11</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA6B8136-F534-47F0-91BF-B5A13A50CB7C}">
+  <dimension ref="A1:N11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="14" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9ADDE57-AF66-423D-98D6-81936002DC42}">
+  <dimension ref="A1:N11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="14" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D7C6862-1CB3-49B2-9D7C-8BD8BF37C257}">
+  <dimension ref="A1:N11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="14" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1043,62 +1534,62 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10AB0793-6B76-4209-907D-B54AADB18679}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1106,55 +1597,55 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <f>Ballantyne!C2+Denver!C2+Huntersville!C2+Matthews!C2+'Rock Hill'!C2+Southpark!C2</f>
+        <f>Ballantyne!C2+Denver!C2+FortMill!C2+Huntersville!C2+Matthews!C2+'Rock Hill'!C2+Southpark!C2</f>
         <v>0</v>
       </c>
       <c r="D2">
-        <f>Ballantyne!D2+Denver!D2+Huntersville!D2+Matthews!D2+'Rock Hill'!D2+Southpark!D2</f>
+        <f>Ballantyne!D2+Denver!D2+FortMill!D2+Huntersville!D2+Matthews!D2+'Rock Hill'!D2+Southpark!D2</f>
         <v>0</v>
       </c>
       <c r="E2">
-        <f>Ballantyne!E2+Denver!E2+Huntersville!E2+Matthews!E2+'Rock Hill'!E2+Southpark!E2</f>
+        <f>Ballantyne!E2+Denver!E2+FortMill!E2+Huntersville!E2+Matthews!E2+'Rock Hill'!E2+Southpark!E2</f>
         <v>0</v>
       </c>
       <c r="F2">
-        <f>Ballantyne!F2+Denver!F2+Huntersville!F2+Matthews!F2+'Rock Hill'!F2+Southpark!F2</f>
+        <f>Ballantyne!F2+Denver!F2+FortMill!F2+Huntersville!F2+Matthews!F2+'Rock Hill'!F2+Southpark!F2</f>
         <v>0</v>
       </c>
       <c r="G2">
-        <f>Ballantyne!G2+Denver!G2+Huntersville!G2+Matthews!G2+'Rock Hill'!G2+Southpark!G2</f>
+        <f>Ballantyne!G2+Denver!G2+FortMill!G2+Huntersville!G2+Matthews!G2+'Rock Hill'!G2+Southpark!G2</f>
         <v>0</v>
       </c>
       <c r="H2">
-        <f>Ballantyne!H2+Denver!H2+Huntersville!H2+Matthews!H2+'Rock Hill'!H2+Southpark!H2</f>
+        <f>Ballantyne!H2+Denver!H2+FortMill!H2+Huntersville!H2+Matthews!H2+'Rock Hill'!H2+Southpark!H2</f>
         <v>0</v>
       </c>
       <c r="I2">
-        <f>Ballantyne!I2+Denver!I2+Huntersville!I2+Matthews!I2+'Rock Hill'!I2+Southpark!I2</f>
+        <f>Ballantyne!I2+Denver!I2+FortMill!I2+Huntersville!I2+Matthews!I2+'Rock Hill'!I2+Southpark!I2</f>
         <v>0</v>
       </c>
       <c r="J2">
-        <f>Ballantyne!J2+Denver!J2+Huntersville!J2+Matthews!J2+'Rock Hill'!J2+Southpark!J2</f>
+        <f>Ballantyne!J2+Denver!J2+FortMill!J2+Huntersville!J2+Matthews!J2+'Rock Hill'!J2+Southpark!J2</f>
         <v>0</v>
       </c>
       <c r="K2">
-        <f>Ballantyne!K2+Denver!K2+Huntersville!K2+Matthews!K2+'Rock Hill'!K2+Southpark!K2</f>
+        <f>Ballantyne!K2+Denver!K2+FortMill!K2+Huntersville!K2+Matthews!K2+'Rock Hill'!K2+Southpark!K2</f>
         <v>0</v>
       </c>
       <c r="L2">
-        <f>Ballantyne!L2+Denver!L2+Huntersville!L2+Matthews!L2+'Rock Hill'!L2+Southpark!L2</f>
+        <f>Ballantyne!L2+Denver!L2+FortMill!L2+Huntersville!L2+Matthews!L2+'Rock Hill'!L2+Southpark!L2</f>
         <v>0</v>
       </c>
       <c r="M2">
-        <f>Ballantyne!M2+Denver!M2+Huntersville!M2+Matthews!M2+'Rock Hill'!M2+Southpark!M2</f>
+        <f>Ballantyne!M2+Denver!M2+FortMill!M2+Huntersville!M2+Matthews!M2+'Rock Hill'!M2+Southpark!M2</f>
         <v>0</v>
       </c>
       <c r="N2">
-        <f>Ballantyne!N2+Denver!N2+Huntersville!N2+Matthews!N2+'Rock Hill'!N2+Southpark!N2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+        <f>Ballantyne!N2+Denver!N2+FortMill!N2+Huntersville!N2+Matthews!N2+'Rock Hill'!N2+Southpark!N2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1162,55 +1653,55 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <f>Ballantyne!C3+Denver!C3+Huntersville!C3+Matthews!C3+'Rock Hill'!C3+Southpark!C3</f>
+        <f>Ballantyne!C3+Denver!C3+FortMill!C3+Huntersville!C3+Matthews!C3+'Rock Hill'!C3+Southpark!C3</f>
         <v>0</v>
       </c>
       <c r="D3">
-        <f>Ballantyne!D3+Denver!D3+Huntersville!D3+Matthews!D3+'Rock Hill'!D3+Southpark!D3</f>
+        <f>Ballantyne!D3+Denver!D3+FortMill!D3+Huntersville!D3+Matthews!D3+'Rock Hill'!D3+Southpark!D3</f>
         <v>0</v>
       </c>
       <c r="E3">
-        <f>Ballantyne!E3+Denver!E3+Huntersville!E3+Matthews!E3+'Rock Hill'!E3+Southpark!E3</f>
+        <f>Ballantyne!E3+Denver!E3+FortMill!E3+Huntersville!E3+Matthews!E3+'Rock Hill'!E3+Southpark!E3</f>
         <v>0</v>
       </c>
       <c r="F3">
-        <f>Ballantyne!F3+Denver!F3+Huntersville!F3+Matthews!F3+'Rock Hill'!F3+Southpark!F3</f>
+        <f>Ballantyne!F3+Denver!F3+FortMill!F3+Huntersville!F3+Matthews!F3+'Rock Hill'!F3+Southpark!F3</f>
         <v>0</v>
       </c>
       <c r="G3">
-        <f>Ballantyne!G3+Denver!G3+Huntersville!G3+Matthews!G3+'Rock Hill'!G3+Southpark!G3</f>
+        <f>Ballantyne!G3+Denver!G3+FortMill!G3+Huntersville!G3+Matthews!G3+'Rock Hill'!G3+Southpark!G3</f>
         <v>0</v>
       </c>
       <c r="H3">
-        <f>Ballantyne!H3+Denver!H3+Huntersville!H3+Matthews!H3+'Rock Hill'!H3+Southpark!H3</f>
+        <f>Ballantyne!H3+Denver!H3+FortMill!H3+Huntersville!H3+Matthews!H3+'Rock Hill'!H3+Southpark!H3</f>
         <v>0</v>
       </c>
       <c r="I3">
-        <f>Ballantyne!I3+Denver!I3+Huntersville!I3+Matthews!I3+'Rock Hill'!I3+Southpark!I3</f>
+        <f>Ballantyne!I3+Denver!I3+FortMill!I3+Huntersville!I3+Matthews!I3+'Rock Hill'!I3+Southpark!I3</f>
         <v>0</v>
       </c>
       <c r="J3">
-        <f>Ballantyne!J3+Denver!J3+Huntersville!J3+Matthews!J3+'Rock Hill'!J3+Southpark!J3</f>
+        <f>Ballantyne!J3+Denver!J3+FortMill!J3+Huntersville!J3+Matthews!J3+'Rock Hill'!J3+Southpark!J3</f>
         <v>0</v>
       </c>
       <c r="K3">
-        <f>Ballantyne!K3+Denver!K3+Huntersville!K3+Matthews!K3+'Rock Hill'!K3+Southpark!K3</f>
+        <f>Ballantyne!K3+Denver!K3+FortMill!K3+Huntersville!K3+Matthews!K3+'Rock Hill'!K3+Southpark!K3</f>
         <v>0</v>
       </c>
       <c r="L3">
-        <f>Ballantyne!L3+Denver!L3+Huntersville!L3+Matthews!L3+'Rock Hill'!L3+Southpark!L3</f>
+        <f>Ballantyne!L3+Denver!L3+FortMill!L3+Huntersville!L3+Matthews!L3+'Rock Hill'!L3+Southpark!L3</f>
         <v>0</v>
       </c>
       <c r="M3">
-        <f>Ballantyne!M3+Denver!M3+Huntersville!M3+Matthews!M3+'Rock Hill'!M3+Southpark!M3</f>
+        <f>Ballantyne!M3+Denver!M3+FortMill!M3+Huntersville!M3+Matthews!M3+'Rock Hill'!M3+Southpark!M3</f>
         <v>0</v>
       </c>
       <c r="N3">
-        <f>Ballantyne!N3+Denver!N3+Huntersville!N3+Matthews!N3+'Rock Hill'!N3+Southpark!N3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+        <f>Ballantyne!N3+Denver!N3+FortMill!N3+Huntersville!N3+Matthews!N3+'Rock Hill'!N3+Southpark!N3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1218,55 +1709,55 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <f>Ballantyne!C4+Denver!C4+Huntersville!C4+Matthews!C4+'Rock Hill'!C4+Southpark!C4</f>
+        <f>Ballantyne!C4+Denver!C4+FortMill!C4+Huntersville!C4+Matthews!C4+'Rock Hill'!C4+Southpark!C4</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f>Ballantyne!D4+Denver!D4+Huntersville!D4+Matthews!D4+'Rock Hill'!D4+Southpark!D4</f>
+        <f>Ballantyne!D4+Denver!D4+FortMill!D4+Huntersville!D4+Matthews!D4+'Rock Hill'!D4+Southpark!D4</f>
         <v>0</v>
       </c>
       <c r="E4">
-        <f>Ballantyne!E4+Denver!E4+Huntersville!E4+Matthews!E4+'Rock Hill'!E4+Southpark!E4</f>
+        <f>Ballantyne!E4+Denver!E4+FortMill!E4+Huntersville!E4+Matthews!E4+'Rock Hill'!E4+Southpark!E4</f>
         <v>0</v>
       </c>
       <c r="F4">
-        <f>Ballantyne!F4+Denver!F4+Huntersville!F4+Matthews!F4+'Rock Hill'!F4+Southpark!F4</f>
+        <f>Ballantyne!F4+Denver!F4+FortMill!F4+Huntersville!F4+Matthews!F4+'Rock Hill'!F4+Southpark!F4</f>
         <v>0</v>
       </c>
       <c r="G4">
-        <f>Ballantyne!G4+Denver!G4+Huntersville!G4+Matthews!G4+'Rock Hill'!G4+Southpark!G4</f>
+        <f>Ballantyne!G4+Denver!G4+FortMill!G4+Huntersville!G4+Matthews!G4+'Rock Hill'!G4+Southpark!G4</f>
         <v>0</v>
       </c>
       <c r="H4">
-        <f>Ballantyne!H4+Denver!H4+Huntersville!H4+Matthews!H4+'Rock Hill'!H4+Southpark!H4</f>
+        <f>Ballantyne!H4+Denver!H4+FortMill!H4+Huntersville!H4+Matthews!H4+'Rock Hill'!H4+Southpark!H4</f>
         <v>0</v>
       </c>
       <c r="I4">
-        <f>Ballantyne!I4+Denver!I4+Huntersville!I4+Matthews!I4+'Rock Hill'!I4+Southpark!I4</f>
+        <f>Ballantyne!I4+Denver!I4+FortMill!I4+Huntersville!I4+Matthews!I4+'Rock Hill'!I4+Southpark!I4</f>
         <v>0</v>
       </c>
       <c r="J4">
-        <f>Ballantyne!J4+Denver!J4+Huntersville!J4+Matthews!J4+'Rock Hill'!J4+Southpark!J4</f>
+        <f>Ballantyne!J4+Denver!J4+FortMill!J4+Huntersville!J4+Matthews!J4+'Rock Hill'!J4+Southpark!J4</f>
         <v>0</v>
       </c>
       <c r="K4">
-        <f>Ballantyne!K4+Denver!K4+Huntersville!K4+Matthews!K4+'Rock Hill'!K4+Southpark!K4</f>
+        <f>Ballantyne!K4+Denver!K4+FortMill!K4+Huntersville!K4+Matthews!K4+'Rock Hill'!K4+Southpark!K4</f>
         <v>0</v>
       </c>
       <c r="L4">
-        <f>Ballantyne!L4+Denver!L4+Huntersville!L4+Matthews!L4+'Rock Hill'!L4+Southpark!L4</f>
+        <f>Ballantyne!L4+Denver!L4+FortMill!L4+Huntersville!L4+Matthews!L4+'Rock Hill'!L4+Southpark!L4</f>
         <v>0</v>
       </c>
       <c r="M4">
-        <f>Ballantyne!M4+Denver!M4+Huntersville!M4+Matthews!M4+'Rock Hill'!M4+Southpark!M4</f>
+        <f>Ballantyne!M4+Denver!M4+FortMill!M4+Huntersville!M4+Matthews!M4+'Rock Hill'!M4+Southpark!M4</f>
         <v>0</v>
       </c>
       <c r="N4">
-        <f>Ballantyne!N4+Denver!N4+Huntersville!N4+Matthews!N4+'Rock Hill'!N4+Southpark!N4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+        <f>Ballantyne!N4+Denver!N4+FortMill!N4+Huntersville!N4+Matthews!N4+'Rock Hill'!N4+Southpark!N4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1274,55 +1765,55 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <f>Ballantyne!C5+Denver!C5+Huntersville!C5+Matthews!C5+'Rock Hill'!C5+Southpark!C5</f>
+        <f>Ballantyne!C5+Denver!C5+FortMill!C5+Huntersville!C5+Matthews!C5+'Rock Hill'!C5+Southpark!C5</f>
         <v>0</v>
       </c>
       <c r="D5">
-        <f>Ballantyne!D5+Denver!D5+Huntersville!D5+Matthews!D5+'Rock Hill'!D5+Southpark!D5</f>
+        <f>Ballantyne!D5+Denver!D5+FortMill!D5+Huntersville!D5+Matthews!D5+'Rock Hill'!D5+Southpark!D5</f>
         <v>0</v>
       </c>
       <c r="E5">
-        <f>Ballantyne!E5+Denver!E5+Huntersville!E5+Matthews!E5+'Rock Hill'!E5+Southpark!E5</f>
+        <f>Ballantyne!E5+Denver!E5+FortMill!E5+Huntersville!E5+Matthews!E5+'Rock Hill'!E5+Southpark!E5</f>
         <v>0</v>
       </c>
       <c r="F5">
-        <f>Ballantyne!F5+Denver!F5+Huntersville!F5+Matthews!F5+'Rock Hill'!F5+Southpark!F5</f>
+        <f>Ballantyne!F5+Denver!F5+FortMill!F5+Huntersville!F5+Matthews!F5+'Rock Hill'!F5+Southpark!F5</f>
         <v>0</v>
       </c>
       <c r="G5">
-        <f>Ballantyne!G5+Denver!G5+Huntersville!G5+Matthews!G5+'Rock Hill'!G5+Southpark!G5</f>
+        <f>Ballantyne!G5+Denver!G5+FortMill!G5+Huntersville!G5+Matthews!G5+'Rock Hill'!G5+Southpark!G5</f>
         <v>0</v>
       </c>
       <c r="H5">
-        <f>Ballantyne!H5+Denver!H5+Huntersville!H5+Matthews!H5+'Rock Hill'!H5+Southpark!H5</f>
+        <f>Ballantyne!H5+Denver!H5+FortMill!H5+Huntersville!H5+Matthews!H5+'Rock Hill'!H5+Southpark!H5</f>
         <v>0</v>
       </c>
       <c r="I5">
-        <f>Ballantyne!I5+Denver!I5+Huntersville!I5+Matthews!I5+'Rock Hill'!I5+Southpark!I5</f>
+        <f>Ballantyne!I5+Denver!I5+FortMill!I5+Huntersville!I5+Matthews!I5+'Rock Hill'!I5+Southpark!I5</f>
         <v>0</v>
       </c>
       <c r="J5">
-        <f>Ballantyne!J5+Denver!J5+Huntersville!J5+Matthews!J5+'Rock Hill'!J5+Southpark!J5</f>
+        <f>Ballantyne!J5+Denver!J5+FortMill!J5+Huntersville!J5+Matthews!J5+'Rock Hill'!J5+Southpark!J5</f>
         <v>0</v>
       </c>
       <c r="K5">
-        <f>Ballantyne!K5+Denver!K5+Huntersville!K5+Matthews!K5+'Rock Hill'!K5+Southpark!K5</f>
+        <f>Ballantyne!K5+Denver!K5+FortMill!K5+Huntersville!K5+Matthews!K5+'Rock Hill'!K5+Southpark!K5</f>
         <v>0</v>
       </c>
       <c r="L5">
-        <f>Ballantyne!L5+Denver!L5+Huntersville!L5+Matthews!L5+'Rock Hill'!L5+Southpark!L5</f>
+        <f>Ballantyne!L5+Denver!L5+FortMill!L5+Huntersville!L5+Matthews!L5+'Rock Hill'!L5+Southpark!L5</f>
         <v>0</v>
       </c>
       <c r="M5">
-        <f>Ballantyne!M5+Denver!M5+Huntersville!M5+Matthews!M5+'Rock Hill'!M5+Southpark!M5</f>
+        <f>Ballantyne!M5+Denver!M5+FortMill!M5+Huntersville!M5+Matthews!M5+'Rock Hill'!M5+Southpark!M5</f>
         <v>0</v>
       </c>
       <c r="N5">
-        <f>Ballantyne!N5+Denver!N5+Huntersville!N5+Matthews!N5+'Rock Hill'!N5+Southpark!N5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <f>Ballantyne!N5+Denver!N5+FortMill!N5+Huntersville!N5+Matthews!N5+'Rock Hill'!N5+Southpark!N5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1330,55 +1821,55 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <f>Ballantyne!C6+Denver!C6+Huntersville!C6+Matthews!C6+'Rock Hill'!C6+Southpark!C6</f>
+        <f>Ballantyne!C6+Denver!C6+FortMill!C6+Huntersville!C6+Matthews!C6+'Rock Hill'!C6+Southpark!C6</f>
         <v>0</v>
       </c>
       <c r="D6">
-        <f>Ballantyne!D6+Denver!D6+Huntersville!D6+Matthews!D6+'Rock Hill'!D6+Southpark!D6</f>
+        <f>Ballantyne!D6+Denver!D6+FortMill!D6+Huntersville!D6+Matthews!D6+'Rock Hill'!D6+Southpark!D6</f>
         <v>0</v>
       </c>
       <c r="E6">
-        <f>Ballantyne!E6+Denver!E6+Huntersville!E6+Matthews!E6+'Rock Hill'!E6+Southpark!E6</f>
+        <f>Ballantyne!E6+Denver!E6+FortMill!E6+Huntersville!E6+Matthews!E6+'Rock Hill'!E6+Southpark!E6</f>
         <v>0</v>
       </c>
       <c r="F6">
-        <f>Ballantyne!F6+Denver!F6+Huntersville!F6+Matthews!F6+'Rock Hill'!F6+Southpark!F6</f>
+        <f>Ballantyne!F6+Denver!F6+FortMill!F6+Huntersville!F6+Matthews!F6+'Rock Hill'!F6+Southpark!F6</f>
         <v>0</v>
       </c>
       <c r="G6">
-        <f>Ballantyne!G6+Denver!G6+Huntersville!G6+Matthews!G6+'Rock Hill'!G6+Southpark!G6</f>
+        <f>Ballantyne!G6+Denver!G6+FortMill!G6+Huntersville!G6+Matthews!G6+'Rock Hill'!G6+Southpark!G6</f>
         <v>0</v>
       </c>
       <c r="H6">
-        <f>Ballantyne!H6+Denver!H6+Huntersville!H6+Matthews!H6+'Rock Hill'!H6+Southpark!H6</f>
+        <f>Ballantyne!H6+Denver!H6+FortMill!H6+Huntersville!H6+Matthews!H6+'Rock Hill'!H6+Southpark!H6</f>
         <v>0</v>
       </c>
       <c r="I6">
-        <f>Ballantyne!I6+Denver!I6+Huntersville!I6+Matthews!I6+'Rock Hill'!I6+Southpark!I6</f>
+        <f>Ballantyne!I6+Denver!I6+FortMill!I6+Huntersville!I6+Matthews!I6+'Rock Hill'!I6+Southpark!I6</f>
         <v>0</v>
       </c>
       <c r="J6">
-        <f>Ballantyne!J6+Denver!J6+Huntersville!J6+Matthews!J6+'Rock Hill'!J6+Southpark!J6</f>
+        <f>Ballantyne!J6+Denver!J6+FortMill!J6+Huntersville!J6+Matthews!J6+'Rock Hill'!J6+Southpark!J6</f>
         <v>0</v>
       </c>
       <c r="K6">
-        <f>Ballantyne!K6+Denver!K6+Huntersville!K6+Matthews!K6+'Rock Hill'!K6+Southpark!K6</f>
+        <f>Ballantyne!K6+Denver!K6+FortMill!K6+Huntersville!K6+Matthews!K6+'Rock Hill'!K6+Southpark!K6</f>
         <v>0</v>
       </c>
       <c r="L6">
-        <f>Ballantyne!L6+Denver!L6+Huntersville!L6+Matthews!L6+'Rock Hill'!L6+Southpark!L6</f>
+        <f>Ballantyne!L6+Denver!L6+FortMill!L6+Huntersville!L6+Matthews!L6+'Rock Hill'!L6+Southpark!L6</f>
         <v>0</v>
       </c>
       <c r="M6">
-        <f>Ballantyne!M6+Denver!M6+Huntersville!M6+Matthews!M6+'Rock Hill'!M6+Southpark!M6</f>
+        <f>Ballantyne!M6+Denver!M6+FortMill!M6+Huntersville!M6+Matthews!M6+'Rock Hill'!M6+Southpark!M6</f>
         <v>0</v>
       </c>
       <c r="N6">
-        <f>Ballantyne!N6+Denver!N6+Huntersville!N6+Matthews!N6+'Rock Hill'!N6+Southpark!N6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+        <f>Ballantyne!N6+Denver!N6+FortMill!N6+Huntersville!N6+Matthews!N6+'Rock Hill'!N6+Southpark!N6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1386,55 +1877,55 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <f>Ballantyne!C7+Denver!C7+Huntersville!C7+Matthews!C7+'Rock Hill'!C7+Southpark!C7</f>
+        <f>Ballantyne!C7+Denver!C7+FortMill!C7+Huntersville!C7+Matthews!C7+'Rock Hill'!C7+Southpark!C7</f>
         <v>0</v>
       </c>
       <c r="D7">
-        <f>Ballantyne!D7+Denver!D7+Huntersville!D7+Matthews!D7+'Rock Hill'!D7+Southpark!D7</f>
+        <f>Ballantyne!D7+Denver!D7+FortMill!D7+Huntersville!D7+Matthews!D7+'Rock Hill'!D7+Southpark!D7</f>
         <v>0</v>
       </c>
       <c r="E7">
-        <f>Ballantyne!E7+Denver!E7+Huntersville!E7+Matthews!E7+'Rock Hill'!E7+Southpark!E7</f>
+        <f>Ballantyne!E7+Denver!E7+FortMill!E7+Huntersville!E7+Matthews!E7+'Rock Hill'!E7+Southpark!E7</f>
         <v>0</v>
       </c>
       <c r="F7">
-        <f>Ballantyne!F7+Denver!F7+Huntersville!F7+Matthews!F7+'Rock Hill'!F7+Southpark!F7</f>
+        <f>Ballantyne!F7+Denver!F7+FortMill!F7+Huntersville!F7+Matthews!F7+'Rock Hill'!F7+Southpark!F7</f>
         <v>0</v>
       </c>
       <c r="G7">
-        <f>Ballantyne!G7+Denver!G7+Huntersville!G7+Matthews!G7+'Rock Hill'!G7+Southpark!G7</f>
+        <f>Ballantyne!G7+Denver!G7+FortMill!G7+Huntersville!G7+Matthews!G7+'Rock Hill'!G7+Southpark!G7</f>
         <v>0</v>
       </c>
       <c r="H7">
-        <f>Ballantyne!H7+Denver!H7+Huntersville!H7+Matthews!H7+'Rock Hill'!H7+Southpark!H7</f>
+        <f>Ballantyne!H7+Denver!H7+FortMill!H7+Huntersville!H7+Matthews!H7+'Rock Hill'!H7+Southpark!H7</f>
         <v>0</v>
       </c>
       <c r="I7">
-        <f>Ballantyne!I7+Denver!I7+Huntersville!I7+Matthews!I7+'Rock Hill'!I7+Southpark!I7</f>
+        <f>Ballantyne!I7+Denver!I7+FortMill!I7+Huntersville!I7+Matthews!I7+'Rock Hill'!I7+Southpark!I7</f>
         <v>0</v>
       </c>
       <c r="J7">
-        <f>Ballantyne!J7+Denver!J7+Huntersville!J7+Matthews!J7+'Rock Hill'!J7+Southpark!J7</f>
+        <f>Ballantyne!J7+Denver!J7+FortMill!J7+Huntersville!J7+Matthews!J7+'Rock Hill'!J7+Southpark!J7</f>
         <v>0</v>
       </c>
       <c r="K7">
-        <f>Ballantyne!K7+Denver!K7+Huntersville!K7+Matthews!K7+'Rock Hill'!K7+Southpark!K7</f>
+        <f>Ballantyne!K7+Denver!K7+FortMill!K7+Huntersville!K7+Matthews!K7+'Rock Hill'!K7+Southpark!K7</f>
         <v>0</v>
       </c>
       <c r="L7">
-        <f>Ballantyne!L7+Denver!L7+Huntersville!L7+Matthews!L7+'Rock Hill'!L7+Southpark!L7</f>
+        <f>Ballantyne!L7+Denver!L7+FortMill!L7+Huntersville!L7+Matthews!L7+'Rock Hill'!L7+Southpark!L7</f>
         <v>0</v>
       </c>
       <c r="M7">
-        <f>Ballantyne!M7+Denver!M7+Huntersville!M7+Matthews!M7+'Rock Hill'!M7+Southpark!M7</f>
+        <f>Ballantyne!M7+Denver!M7+FortMill!M7+Huntersville!M7+Matthews!M7+'Rock Hill'!M7+Southpark!M7</f>
         <v>0</v>
       </c>
       <c r="N7">
-        <f>Ballantyne!N7+Denver!N7+Huntersville!N7+Matthews!N7+'Rock Hill'!N7+Southpark!N7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+        <f>Ballantyne!N7+Denver!N7+FortMill!N7+Huntersville!N7+Matthews!N7+'Rock Hill'!N7+Southpark!N7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1442,55 +1933,55 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <f>Ballantyne!C8+Denver!C8+Huntersville!C8+Matthews!C8+'Rock Hill'!C8+Southpark!C8</f>
+        <f>Ballantyne!C8+Denver!C8+FortMill!C8+Huntersville!C8+Matthews!C8+'Rock Hill'!C8+Southpark!C8</f>
         <v>0</v>
       </c>
       <c r="D8">
-        <f>Ballantyne!D8+Denver!D8+Huntersville!D8+Matthews!D8+'Rock Hill'!D8+Southpark!D8</f>
+        <f>Ballantyne!D8+Denver!D8+FortMill!D8+Huntersville!D8+Matthews!D8+'Rock Hill'!D8+Southpark!D8</f>
         <v>0</v>
       </c>
       <c r="E8">
-        <f>Ballantyne!E8+Denver!E8+Huntersville!E8+Matthews!E8+'Rock Hill'!E8+Southpark!E8</f>
+        <f>Ballantyne!E8+Denver!E8+FortMill!E8+Huntersville!E8+Matthews!E8+'Rock Hill'!E8+Southpark!E8</f>
         <v>0</v>
       </c>
       <c r="F8">
-        <f>Ballantyne!F8+Denver!F8+Huntersville!F8+Matthews!F8+'Rock Hill'!F8+Southpark!F8</f>
+        <f>Ballantyne!F8+Denver!F8+FortMill!F8+Huntersville!F8+Matthews!F8+'Rock Hill'!F8+Southpark!F8</f>
         <v>0</v>
       </c>
       <c r="G8">
-        <f>Ballantyne!G8+Denver!G8+Huntersville!G8+Matthews!G8+'Rock Hill'!G8+Southpark!G8</f>
+        <f>Ballantyne!G8+Denver!G8+FortMill!G8+Huntersville!G8+Matthews!G8+'Rock Hill'!G8+Southpark!G8</f>
         <v>0</v>
       </c>
       <c r="H8">
-        <f>Ballantyne!H8+Denver!H8+Huntersville!H8+Matthews!H8+'Rock Hill'!H8+Southpark!H8</f>
+        <f>Ballantyne!H8+Denver!H8+FortMill!H8+Huntersville!H8+Matthews!H8+'Rock Hill'!H8+Southpark!H8</f>
         <v>0</v>
       </c>
       <c r="I8">
-        <f>Ballantyne!I8+Denver!I8+Huntersville!I8+Matthews!I8+'Rock Hill'!I8+Southpark!I8</f>
+        <f>Ballantyne!I8+Denver!I8+FortMill!I8+Huntersville!I8+Matthews!I8+'Rock Hill'!I8+Southpark!I8</f>
         <v>0</v>
       </c>
       <c r="J8">
-        <f>Ballantyne!J8+Denver!J8+Huntersville!J8+Matthews!J8+'Rock Hill'!J8+Southpark!J8</f>
+        <f>Ballantyne!J8+Denver!J8+FortMill!J8+Huntersville!J8+Matthews!J8+'Rock Hill'!J8+Southpark!J8</f>
         <v>0</v>
       </c>
       <c r="K8">
-        <f>Ballantyne!K8+Denver!K8+Huntersville!K8+Matthews!K8+'Rock Hill'!K8+Southpark!K8</f>
+        <f>Ballantyne!K8+Denver!K8+FortMill!K8+Huntersville!K8+Matthews!K8+'Rock Hill'!K8+Southpark!K8</f>
         <v>0</v>
       </c>
       <c r="L8">
-        <f>Ballantyne!L8+Denver!L8+Huntersville!L8+Matthews!L8+'Rock Hill'!L8+Southpark!L8</f>
+        <f>Ballantyne!L8+Denver!L8+FortMill!L8+Huntersville!L8+Matthews!L8+'Rock Hill'!L8+Southpark!L8</f>
         <v>0</v>
       </c>
       <c r="M8">
-        <f>Ballantyne!M8+Denver!M8+Huntersville!M8+Matthews!M8+'Rock Hill'!M8+Southpark!M8</f>
+        <f>Ballantyne!M8+Denver!M8+FortMill!M8+Huntersville!M8+Matthews!M8+'Rock Hill'!M8+Southpark!M8</f>
         <v>0</v>
       </c>
       <c r="N8">
-        <f>Ballantyne!N8+Denver!N8+Huntersville!N8+Matthews!N8+'Rock Hill'!N8+Southpark!N8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+        <f>Ballantyne!N8+Denver!N8+FortMill!N8+Huntersville!N8+Matthews!N8+'Rock Hill'!N8+Southpark!N8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1498,55 +1989,55 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <f>Ballantyne!C9+Denver!C9+Huntersville!C9+Matthews!C9+'Rock Hill'!C9+Southpark!C9</f>
+        <f>Ballantyne!C9+Denver!C9+FortMill!C9+Huntersville!C9+Matthews!C9+'Rock Hill'!C9+Southpark!C9</f>
         <v>0</v>
       </c>
       <c r="D9">
-        <f>Ballantyne!D9+Denver!D9+Huntersville!D9+Matthews!D9+'Rock Hill'!D9+Southpark!D9</f>
+        <f>Ballantyne!D9+Denver!D9+FortMill!D9+Huntersville!D9+Matthews!D9+'Rock Hill'!D9+Southpark!D9</f>
         <v>0</v>
       </c>
       <c r="E9">
-        <f>Ballantyne!E9+Denver!E9+Huntersville!E9+Matthews!E9+'Rock Hill'!E9+Southpark!E9</f>
+        <f>Ballantyne!E9+Denver!E9+FortMill!E9+Huntersville!E9+Matthews!E9+'Rock Hill'!E9+Southpark!E9</f>
         <v>0</v>
       </c>
       <c r="F9">
-        <f>Ballantyne!F9+Denver!F9+Huntersville!F9+Matthews!F9+'Rock Hill'!F9+Southpark!F9</f>
+        <f>Ballantyne!F9+Denver!F9+FortMill!F9+Huntersville!F9+Matthews!F9+'Rock Hill'!F9+Southpark!F9</f>
         <v>0</v>
       </c>
       <c r="G9">
-        <f>Ballantyne!G9+Denver!G9+Huntersville!G9+Matthews!G9+'Rock Hill'!G9+Southpark!G9</f>
+        <f>Ballantyne!G9+Denver!G9+FortMill!G9+Huntersville!G9+Matthews!G9+'Rock Hill'!G9+Southpark!G9</f>
         <v>0</v>
       </c>
       <c r="H9">
-        <f>Ballantyne!H9+Denver!H9+Huntersville!H9+Matthews!H9+'Rock Hill'!H9+Southpark!H9</f>
+        <f>Ballantyne!H9+Denver!H9+FortMill!H9+Huntersville!H9+Matthews!H9+'Rock Hill'!H9+Southpark!H9</f>
         <v>0</v>
       </c>
       <c r="I9">
-        <f>Ballantyne!I9+Denver!I9+Huntersville!I9+Matthews!I9+'Rock Hill'!I9+Southpark!I9</f>
+        <f>Ballantyne!I9+Denver!I9+FortMill!I9+Huntersville!I9+Matthews!I9+'Rock Hill'!I9+Southpark!I9</f>
         <v>0</v>
       </c>
       <c r="J9">
-        <f>Ballantyne!J9+Denver!J9+Huntersville!J9+Matthews!J9+'Rock Hill'!J9+Southpark!J9</f>
+        <f>Ballantyne!J9+Denver!J9+FortMill!J9+Huntersville!J9+Matthews!J9+'Rock Hill'!J9+Southpark!J9</f>
         <v>0</v>
       </c>
       <c r="K9">
-        <f>Ballantyne!K9+Denver!K9+Huntersville!K9+Matthews!K9+'Rock Hill'!K9+Southpark!K9</f>
+        <f>Ballantyne!K9+Denver!K9+FortMill!K9+Huntersville!K9+Matthews!K9+'Rock Hill'!K9+Southpark!K9</f>
         <v>0</v>
       </c>
       <c r="L9">
-        <f>Ballantyne!L9+Denver!L9+Huntersville!L9+Matthews!L9+'Rock Hill'!L9+Southpark!L9</f>
+        <f>Ballantyne!L9+Denver!L9+FortMill!L9+Huntersville!L9+Matthews!L9+'Rock Hill'!L9+Southpark!L9</f>
         <v>0</v>
       </c>
       <c r="M9">
-        <f>Ballantyne!M9+Denver!M9+Huntersville!M9+Matthews!M9+'Rock Hill'!M9+Southpark!M9</f>
+        <f>Ballantyne!M9+Denver!M9+FortMill!M9+Huntersville!M9+Matthews!M9+'Rock Hill'!M9+Southpark!M9</f>
         <v>0</v>
       </c>
       <c r="N9">
-        <f>Ballantyne!N9+Denver!N9+Huntersville!N9+Matthews!N9+'Rock Hill'!N9+Southpark!N9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+        <f>Ballantyne!N9+Denver!N9+FortMill!N9+Huntersville!N9+Matthews!N9+'Rock Hill'!N9+Southpark!N9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1554,51 +2045,107 @@
         <v>2</v>
       </c>
       <c r="C10">
-        <f>Ballantyne!C10+Denver!C10+Huntersville!C10+Matthews!C10+'Rock Hill'!C10+Southpark!C10</f>
+        <f>Ballantyne!C10+Denver!C10+FortMill!C10+Huntersville!C10+Matthews!C10+'Rock Hill'!C10+Southpark!C10</f>
         <v>0</v>
       </c>
       <c r="D10">
-        <f>Ballantyne!D10+Denver!D10+Huntersville!D10+Matthews!D10+'Rock Hill'!D10+Southpark!D10</f>
+        <f>Ballantyne!D10+Denver!D10+FortMill!D10+Huntersville!D10+Matthews!D10+'Rock Hill'!D10+Southpark!D10</f>
         <v>0</v>
       </c>
       <c r="E10">
-        <f>Ballantyne!E10+Denver!E10+Huntersville!E10+Matthews!E10+'Rock Hill'!E10+Southpark!E10</f>
+        <f>Ballantyne!E10+Denver!E10+FortMill!E10+Huntersville!E10+Matthews!E10+'Rock Hill'!E10+Southpark!E10</f>
         <v>0</v>
       </c>
       <c r="F10">
-        <f>Ballantyne!F10+Denver!F10+Huntersville!F10+Matthews!F10+'Rock Hill'!F10+Southpark!F10</f>
+        <f>Ballantyne!F10+Denver!F10+FortMill!F10+Huntersville!F10+Matthews!F10+'Rock Hill'!F10+Southpark!F10</f>
         <v>0</v>
       </c>
       <c r="G10">
-        <f>Ballantyne!G10+Denver!G10+Huntersville!G10+Matthews!G10+'Rock Hill'!G10+Southpark!G10</f>
+        <f>Ballantyne!G10+Denver!G10+FortMill!G10+Huntersville!G10+Matthews!G10+'Rock Hill'!G10+Southpark!G10</f>
         <v>0</v>
       </c>
       <c r="H10">
-        <f>Ballantyne!H10+Denver!H10+Huntersville!H10+Matthews!H10+'Rock Hill'!H10+Southpark!H10</f>
+        <f>Ballantyne!H10+Denver!H10+FortMill!H10+Huntersville!H10+Matthews!H10+'Rock Hill'!H10+Southpark!H10</f>
         <v>0</v>
       </c>
       <c r="I10">
-        <f>Ballantyne!I10+Denver!I10+Huntersville!I10+Matthews!I10+'Rock Hill'!I10+Southpark!I10</f>
+        <f>Ballantyne!I10+Denver!I10+FortMill!I10+Huntersville!I10+Matthews!I10+'Rock Hill'!I10+Southpark!I10</f>
         <v>0</v>
       </c>
       <c r="J10">
-        <f>Ballantyne!J10+Denver!J10+Huntersville!J10+Matthews!J10+'Rock Hill'!J10+Southpark!J10</f>
+        <f>Ballantyne!J10+Denver!J10+FortMill!J10+Huntersville!J10+Matthews!J10+'Rock Hill'!J10+Southpark!J10</f>
         <v>0</v>
       </c>
       <c r="K10">
-        <f>Ballantyne!K10+Denver!K10+Huntersville!K10+Matthews!K10+'Rock Hill'!K10+Southpark!K10</f>
+        <f>Ballantyne!K10+Denver!K10+FortMill!K10+Huntersville!K10+Matthews!K10+'Rock Hill'!K10+Southpark!K10</f>
         <v>0</v>
       </c>
       <c r="L10">
-        <f>Ballantyne!L10+Denver!L10+Huntersville!L10+Matthews!L10+'Rock Hill'!L10+Southpark!L10</f>
+        <f>Ballantyne!L10+Denver!L10+FortMill!L10+Huntersville!L10+Matthews!L10+'Rock Hill'!L10+Southpark!L10</f>
         <v>0</v>
       </c>
       <c r="M10">
-        <f>Ballantyne!M10+Denver!M10+Huntersville!M10+Matthews!M10+'Rock Hill'!M10+Southpark!M10</f>
+        <f>Ballantyne!M10+Denver!M10+FortMill!M10+Huntersville!M10+Matthews!M10+'Rock Hill'!M10+Southpark!M10</f>
         <v>0</v>
       </c>
       <c r="N10">
-        <f>Ballantyne!N10+Denver!N10+Huntersville!N10+Matthews!N10+'Rock Hill'!N10+Southpark!N10</f>
+        <f>Ballantyne!N10+Denver!N10+FortMill!N10+Huntersville!N10+Matthews!N10+'Rock Hill'!N10+Southpark!N10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <f>Ballantyne!C11+Denver!C11+FortMill!C11+Huntersville!C11+Matthews!C11+'Rock Hill'!C11+Southpark!C11</f>
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f>Ballantyne!D11+Denver!D11+FortMill!D11+Huntersville!D11+Matthews!D11+'Rock Hill'!D11+Southpark!D11</f>
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f>Ballantyne!E11+Denver!E11+FortMill!E11+Huntersville!E11+Matthews!E11+'Rock Hill'!E11+Southpark!E11</f>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f>Ballantyne!F11+Denver!F11+FortMill!F11+Huntersville!F11+Matthews!F11+'Rock Hill'!F11+Southpark!F11</f>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f>Ballantyne!G11+Denver!G11+FortMill!G11+Huntersville!G11+Matthews!G11+'Rock Hill'!G11+Southpark!G11</f>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f>Ballantyne!H11+Denver!H11+FortMill!H11+Huntersville!H11+Matthews!H11+'Rock Hill'!H11+Southpark!H11</f>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f>Ballantyne!I11+Denver!I11+FortMill!I11+Huntersville!I11+Matthews!I11+'Rock Hill'!I11+Southpark!I11</f>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <f>Ballantyne!J11+Denver!J11+FortMill!J11+Huntersville!J11+Matthews!J11+'Rock Hill'!J11+Southpark!J11</f>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <f>Ballantyne!K11+Denver!K11+FortMill!K11+Huntersville!K11+Matthews!K11+'Rock Hill'!K11+Southpark!K11</f>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f>Ballantyne!L11+Denver!L11+FortMill!L11+Huntersville!L11+Matthews!L11+'Rock Hill'!L11+Southpark!L11</f>
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <f>Ballantyne!M11+Denver!M11+FortMill!M11+Huntersville!M11+Matthews!M11+'Rock Hill'!M11+Southpark!M11</f>
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <f>Ballantyne!N11+Denver!N11+FortMill!N11+Huntersville!N11+Matthews!N11+'Rock Hill'!N11+Southpark!N11</f>
         <v>0</v>
       </c>
     </row>
@@ -1609,62 +2156,62 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1672,7 +2219,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1680,7 +2227,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1688,7 +2235,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1696,7 +2243,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1704,7 +2251,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1712,7 +2259,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1720,7 +2267,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1728,12 +2275,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1743,62 +2298,62 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1806,7 +2361,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1814,7 +2369,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1822,7 +2377,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1830,7 +2385,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1838,7 +2393,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1846,7 +2401,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1854,7 +2409,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1862,12 +2417,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1876,63 +2439,63 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:N10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61699067-6179-466C-9D81-CC7465B768B3}">
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1940,7 +2503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1948,7 +2511,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1956,7 +2519,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1964,7 +2527,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1972,7 +2535,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1980,7 +2543,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1988,7 +2551,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1996,12 +2559,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2010,63 +2581,63 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:N10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2074,7 +2645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2082,7 +2653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2090,7 +2661,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2098,7 +2669,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2106,7 +2677,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2114,7 +2685,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2122,7 +2693,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2130,12 +2701,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2144,63 +2723,63 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:N10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2208,7 +2787,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2216,7 +2795,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2224,7 +2803,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2232,7 +2811,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2240,7 +2819,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2248,7 +2827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2256,7 +2835,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2264,12 +2843,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2278,63 +2865,63 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:N10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2342,7 +2929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2350,7 +2937,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2358,7 +2945,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2366,7 +2953,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2374,7 +2961,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2382,7 +2969,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2390,7 +2977,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2398,12 +2985,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2412,63 +3007,63 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61699067-6179-466C-9D81-CC7465B768B3}">
-  <dimension ref="A1:N10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2476,7 +3071,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2484,7 +3079,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2492,7 +3087,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2500,7 +3095,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2508,7 +3103,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2516,7 +3111,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2524,7 +3119,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2532,12 +3127,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Forgot to remove fluoro from CIS strat plan template fml
</commit_message>
<xml_diff>
--- a/CIS_Template_Strat.xlsx
+++ b/CIS_Template_Strat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usradiology-my.sharepoint.com/personal/joshua_mcdonald_usradiology_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0903A04-6BF9-4505-99FE-84648EA2B62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{C0903A04-6BF9-4505-99FE-84648EA2B62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4EDDADB-D3B3-4154-A0BD-30F8E075EC29}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="777" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="777" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary (with DeNovo)" sheetId="22" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="23">
   <si>
     <t>ExamCategory</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>US</t>
-  </si>
-  <si>
-    <t>Fluoroscopy</t>
   </si>
   <si>
     <t>Screening Mamm</t>
@@ -486,7 +483,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B0F8F8-48F1-495E-AB27-ABE4AA2E5916}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -505,40 +502,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -935,10 +932,10 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <f>Ballantyne!C9+Denver!C9+FortMill!C9+Huntersville!C9+Matthews!C9+'Rock Hill'!C9+Southpark!C9+Concord!C9+'Indian Trail'!C9+OtherDeNovo!C9</f>
@@ -991,10 +988,10 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <f>Ballantyne!C10+Denver!C10+FortMill!C10+Huntersville!C10+Matthews!C10+'Rock Hill'!C10+Southpark!C10+Concord!C10+'Indian Trail'!C10+OtherDeNovo!C10</f>
@@ -1042,62 +1039,6 @@
       </c>
       <c r="N10">
         <f>Ballantyne!N10+Denver!N10+FortMill!N10+Huntersville!N10+Matthews!N10+'Rock Hill'!N10+Southpark!N10+Concord!N10+'Indian Trail'!N10+OtherDeNovo!N10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11">
-        <f>Ballantyne!C11+Denver!C11+FortMill!C11+Huntersville!C11+Matthews!C11+'Rock Hill'!C11+Southpark!C11+Concord!C11+'Indian Trail'!C11+OtherDeNovo!C11</f>
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <f>Ballantyne!D11+Denver!D11+FortMill!D11+Huntersville!D11+Matthews!D11+'Rock Hill'!D11+Southpark!D11+Concord!D11+'Indian Trail'!D11+OtherDeNovo!D11</f>
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <f>Ballantyne!E11+Denver!E11+FortMill!E11+Huntersville!E11+Matthews!E11+'Rock Hill'!E11+Southpark!E11+Concord!E11+'Indian Trail'!E11+OtherDeNovo!E11</f>
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <f>Ballantyne!F11+Denver!F11+FortMill!F11+Huntersville!F11+Matthews!F11+'Rock Hill'!F11+Southpark!F11+Concord!F11+'Indian Trail'!F11+OtherDeNovo!F11</f>
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <f>Ballantyne!G11+Denver!G11+FortMill!G11+Huntersville!G11+Matthews!G11+'Rock Hill'!G11+Southpark!G11+Concord!G11+'Indian Trail'!G11+OtherDeNovo!G11</f>
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <f>Ballantyne!H11+Denver!H11+FortMill!H11+Huntersville!H11+Matthews!H11+'Rock Hill'!H11+Southpark!H11+Concord!H11+'Indian Trail'!H11+OtherDeNovo!H11</f>
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <f>Ballantyne!I11+Denver!I11+FortMill!I11+Huntersville!I11+Matthews!I11+'Rock Hill'!I11+Southpark!I11+Concord!I11+'Indian Trail'!I11+OtherDeNovo!I11</f>
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <f>Ballantyne!J11+Denver!J11+FortMill!J11+Huntersville!J11+Matthews!J11+'Rock Hill'!J11+Southpark!J11+Concord!J11+'Indian Trail'!J11+OtherDeNovo!J11</f>
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <f>Ballantyne!K11+Denver!K11+FortMill!K11+Huntersville!K11+Matthews!K11+'Rock Hill'!K11+Southpark!K11+Concord!K11+'Indian Trail'!K11+OtherDeNovo!K11</f>
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <f>Ballantyne!L11+Denver!L11+FortMill!L11+Huntersville!L11+Matthews!L11+'Rock Hill'!L11+Southpark!L11+Concord!L11+'Indian Trail'!L11+OtherDeNovo!L11</f>
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <f>Ballantyne!M11+Denver!M11+FortMill!M11+Huntersville!M11+Matthews!M11+'Rock Hill'!M11+Southpark!M11+Concord!M11+'Indian Trail'!M11+OtherDeNovo!M11</f>
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <f>Ballantyne!N11+Denver!N11+FortMill!N11+Huntersville!N11+Matthews!N11+'Rock Hill'!N11+Southpark!N11+Concord!N11+'Indian Trail'!N11+OtherDeNovo!N11</f>
         <v>0</v>
       </c>
     </row>
@@ -1108,7 +1049,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA6B8136-F534-47F0-91BF-B5A13A50CB7C}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1127,40 +1068,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1221,26 +1162,18 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1250,7 +1183,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9ADDE57-AF66-423D-98D6-81936002DC42}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1269,40 +1202,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1363,26 +1296,18 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1392,7 +1317,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D7C6862-1CB3-49B2-9D7C-8BD8BF37C257}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1411,40 +1336,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1505,26 +1430,18 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1534,7 +1451,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10AB0793-6B76-4209-907D-B54AADB18679}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1553,40 +1470,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1983,10 +1900,10 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <f>Ballantyne!C9+Denver!C9+FortMill!C9+Huntersville!C9+Matthews!C9+'Rock Hill'!C9+Southpark!C9</f>
@@ -2039,10 +1956,10 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <f>Ballantyne!C10+Denver!C10+FortMill!C10+Huntersville!C10+Matthews!C10+'Rock Hill'!C10+Southpark!C10</f>
@@ -2090,62 +2007,6 @@
       </c>
       <c r="N10">
         <f>Ballantyne!N10+Denver!N10+FortMill!N10+Huntersville!N10+Matthews!N10+'Rock Hill'!N10+Southpark!N10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11">
-        <f>Ballantyne!C11+Denver!C11+FortMill!C11+Huntersville!C11+Matthews!C11+'Rock Hill'!C11+Southpark!C11</f>
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <f>Ballantyne!D11+Denver!D11+FortMill!D11+Huntersville!D11+Matthews!D11+'Rock Hill'!D11+Southpark!D11</f>
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <f>Ballantyne!E11+Denver!E11+FortMill!E11+Huntersville!E11+Matthews!E11+'Rock Hill'!E11+Southpark!E11</f>
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <f>Ballantyne!F11+Denver!F11+FortMill!F11+Huntersville!F11+Matthews!F11+'Rock Hill'!F11+Southpark!F11</f>
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <f>Ballantyne!G11+Denver!G11+FortMill!G11+Huntersville!G11+Matthews!G11+'Rock Hill'!G11+Southpark!G11</f>
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <f>Ballantyne!H11+Denver!H11+FortMill!H11+Huntersville!H11+Matthews!H11+'Rock Hill'!H11+Southpark!H11</f>
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <f>Ballantyne!I11+Denver!I11+FortMill!I11+Huntersville!I11+Matthews!I11+'Rock Hill'!I11+Southpark!I11</f>
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <f>Ballantyne!J11+Denver!J11+FortMill!J11+Huntersville!J11+Matthews!J11+'Rock Hill'!J11+Southpark!J11</f>
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <f>Ballantyne!K11+Denver!K11+FortMill!K11+Huntersville!K11+Matthews!K11+'Rock Hill'!K11+Southpark!K11</f>
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <f>Ballantyne!L11+Denver!L11+FortMill!L11+Huntersville!L11+Matthews!L11+'Rock Hill'!L11+Southpark!L11</f>
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <f>Ballantyne!M11+Denver!M11+FortMill!M11+Huntersville!M11+Matthews!M11+'Rock Hill'!M11+Southpark!M11</f>
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <f>Ballantyne!N11+Denver!N11+FortMill!N11+Huntersville!N11+Matthews!N11+'Rock Hill'!N11+Southpark!N11</f>
         <v>0</v>
       </c>
     </row>
@@ -2156,7 +2017,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2175,40 +2036,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -2269,26 +2130,18 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2298,7 +2151,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2317,40 +2170,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -2411,26 +2264,18 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2440,7 +2285,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61699067-6179-466C-9D81-CC7465B768B3}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2459,40 +2304,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -2553,26 +2398,18 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2582,7 +2419,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2601,40 +2438,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -2695,26 +2532,18 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2724,7 +2553,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2743,40 +2572,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -2837,26 +2666,18 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2866,7 +2687,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2885,40 +2706,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -2979,26 +2800,18 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -3008,7 +2821,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3027,40 +2840,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -3121,26 +2934,18 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>